<commit_message>
Add more stats to word count spreadsheets
</commit_message>
<xml_diff>
--- a/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
+++ b/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mark/Documents/Files/Websites/Repositories/bbcelite-scripts/code-analysis/word-count-repositories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mark/Documents/Files/Websites/Repositories/bbcelite-scripts/code-analysis/word-count-code-comments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FB70C1-001F-0849-9E14-6937DADA223F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7681597F-6C35-C24A-8A88-C98F89FB744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="2340" windowWidth="21600" windowHeight="17440" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
+    <workbookView xWindow="11060" yWindow="3020" windowWidth="21600" windowHeight="17440" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="103">
   <si>
     <t>Lines</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>To update the counts, run the script and paste the contents into the linecount.txt and wordcount.txt tabs</t>
+  </si>
+  <si>
+    <t>All Shakespeare's plays</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -415,6 +418,7 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -731,7 +735,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4742C6F-ED5A-B74D-BFAE-09A904247301}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1133,8 +1137,16 @@
         <v>1084625</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="6">
+        <v>835997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1143,6 +1155,7 @@
     <sortCondition descending="1" ref="B2:B11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1150,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A41BAD4-CFE1-7E43-9F45-0738248790D4}">
   <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A73" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Updated line count spreadsheet with latest figures
</commit_message>
<xml_diff>
--- a/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
+++ b/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mark/Documents/Files/Websites/Repositories/bbcelite-scripts/code-analysis/word-count-code-comments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1568A63-8393-0446-A6C3-4F7C6E88B056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B80DC9-781B-334E-8999-B01BA49E7B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16420" yWindow="2820" windowWidth="21600" windowHeight="17440" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
+    <workbookView xWindow="12060" yWindow="2180" windowWidth="21600" windowHeight="17440" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="115">
   <si>
     <t>Lines</t>
   </si>
@@ -341,9 +341,6 @@
     <t>elite-gma2.asm</t>
   </si>
   <si>
-    <t>elite-sprite.asm</t>
-  </si>
-  <si>
     <t>elite-gma3.asm</t>
   </si>
   <si>
@@ -378,6 +375,12 @@
   </si>
   <si>
     <t>elite-a-source-code-6502-second-processor</t>
+  </si>
+  <si>
+    <t>elite-send.asm</t>
+  </si>
+  <si>
+    <t>elite-sprites.asm</t>
   </si>
 </sst>
 </file>
@@ -798,19 +801,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A2,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$I$4</f>
-        <v>151463</v>
+        <v>151582</v>
       </c>
       <c r="C2" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A2)</f>
-        <v>519744</v>
+        <v>520054</v>
       </c>
       <c r="D2" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A2)</f>
-        <v>799871</v>
+        <v>800354</v>
       </c>
       <c r="H2" t="s">
         <v>81</v>
@@ -822,19 +825,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A3,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>113946</v>
+        <v>113986</v>
       </c>
       <c r="C3" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A3)</f>
-        <v>399945</v>
+        <v>400079</v>
       </c>
       <c r="D3" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A3)</f>
-        <v>622084</v>
+        <v>622267</v>
       </c>
       <c r="H3" t="s">
         <v>83</v>
@@ -850,15 +853,15 @@
       </c>
       <c r="B4" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A4,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$I$8</f>
-        <v>100667</v>
+        <v>100795</v>
       </c>
       <c r="C4" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A4)</f>
-        <v>348380</v>
+        <v>348837</v>
       </c>
       <c r="D4" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A4)</f>
-        <v>543079</v>
+        <v>543750</v>
       </c>
       <c r="H4" t="s">
         <v>86</v>
@@ -870,7 +873,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A5,linecount.txt!E:E,"&lt;&gt;revs-build-options.asm",linecount.txt!E:E,"&lt;&gt;revs-disc.asm")</f>
@@ -888,19 +891,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A6,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>65072</v>
+        <v>65989</v>
       </c>
       <c r="C6" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A6)</f>
-        <v>232073</v>
+        <v>246255</v>
       </c>
       <c r="D6" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A6)</f>
-        <v>342861</v>
+        <v>353566</v>
       </c>
       <c r="H6" t="s">
         <v>82</v>
@@ -912,19 +915,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B7" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A7,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>64688</v>
+        <v>65084</v>
       </c>
       <c r="C7" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A7)</f>
-        <v>240504</v>
+        <v>232134</v>
       </c>
       <c r="D7" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A7)</f>
-        <v>346222</v>
+        <v>342936</v>
       </c>
       <c r="H7" t="s">
         <v>85</v>
@@ -940,15 +943,15 @@
       </c>
       <c r="B8" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A8,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>64386</v>
+        <v>64419</v>
       </c>
       <c r="C8" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A8)</f>
-        <v>245393</v>
+        <v>245575</v>
       </c>
       <c r="D8" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A8)</f>
-        <v>354676</v>
+        <v>354905</v>
       </c>
       <c r="H8" t="s">
         <v>86</v>
@@ -960,37 +963,37 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A9,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>59312</v>
+        <v>59341</v>
       </c>
       <c r="C9" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A9)</f>
-        <v>226762</v>
+        <v>226873</v>
       </c>
       <c r="D9" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A9)</f>
-        <v>324068</v>
+        <v>324221</v>
       </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A10,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>52608</v>
+        <v>52672</v>
       </c>
       <c r="C10" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A10)</f>
-        <v>177609</v>
+        <v>177860</v>
       </c>
       <c r="D10" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A10)</f>
-        <v>263637</v>
+        <v>263964</v>
       </c>
       <c r="H10" t="s">
         <v>84</v>
@@ -1003,15 +1006,15 @@
       </c>
       <c r="B11" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A11,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>41758</v>
+        <v>41776</v>
       </c>
       <c r="C11" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A11)</f>
-        <v>171385</v>
+        <v>171489</v>
       </c>
       <c r="D11" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A11)</f>
-        <v>232100</v>
+        <v>232255</v>
       </c>
       <c r="H11" t="s">
         <v>2</v>
@@ -1027,15 +1030,15 @@
       </c>
       <c r="B12" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A12,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>37409</v>
+        <v>37424</v>
       </c>
       <c r="C12" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A12)</f>
-        <v>150404</v>
+        <v>150496</v>
       </c>
       <c r="D12" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A12)</f>
-        <v>204976</v>
+        <v>205103</v>
       </c>
       <c r="H12" t="s">
         <v>8</v>
@@ -1047,7 +1050,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A13,linecount.txt!E:E,"&lt;&gt;aviator-build-options.asm",linecount.txt!E:E,"&lt;&gt;aviator-disc.asm",linecount.txt!E:E,"&lt;&gt;aviator-readme.asm")</f>
@@ -1064,7 +1067,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A14,linecount.txt!E:E,"&lt;&gt;revs-build-options.asm",linecount.txt!E:E,"&lt;&gt;revs-disc.asm")</f>
@@ -1082,15 +1085,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5">
         <f>SUM(B2:B14)</f>
-        <v>865490</v>
+        <v>867249</v>
       </c>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>3168504</v>
+        <v>3175957</v>
       </c>
       <c r="D15" s="5">
         <f>SUM(D2:D14)</f>
-        <v>4664292</v>
+        <v>4674039</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1228,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A41BAD4-CFE1-7E43-9F45-0738248790D4}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E133"/>
+      <selection sqref="A1:E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1243,13 +1246,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B1" s="2">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="C1" s="2">
-        <v>1793</v>
+        <v>1997</v>
       </c>
       <c r="D1" t="s">
         <v>94</v>
@@ -1260,13 +1263,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="B2" s="2">
-        <v>999</v>
+        <v>1041</v>
       </c>
       <c r="C2" s="2">
-        <v>7770</v>
+        <v>8058</v>
       </c>
       <c r="D2" t="s">
         <v>94</v>
@@ -1294,13 +1297,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>38152</v>
+        <v>38158</v>
       </c>
       <c r="B4" s="2">
-        <v>212567</v>
+        <v>212605</v>
       </c>
       <c r="C4" s="2">
-        <v>1474767</v>
+        <v>1475037</v>
       </c>
       <c r="D4" t="s">
         <v>94</v>
@@ -1311,13 +1314,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="C5" s="2">
-        <v>2218</v>
+        <v>2419</v>
       </c>
       <c r="D5" t="s">
         <v>94</v>
@@ -1328,13 +1331,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>3362</v>
+        <v>3367</v>
       </c>
       <c r="B6" s="2">
-        <v>18063</v>
+        <v>18088</v>
       </c>
       <c r="C6" s="2">
-        <v>124836</v>
+        <v>125040</v>
       </c>
       <c r="D6" t="s">
         <v>94</v>
@@ -1345,13 +1348,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>1323</v>
+        <v>1328</v>
       </c>
       <c r="B7" s="2">
-        <v>8405</v>
+        <v>8428</v>
       </c>
       <c r="C7" s="2">
-        <v>60781</v>
+        <v>60970</v>
       </c>
       <c r="D7" t="s">
         <v>95</v>
@@ -1362,13 +1365,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>1377</v>
+        <v>1382</v>
       </c>
       <c r="B8" s="2">
-        <v>8682</v>
+        <v>8705</v>
       </c>
       <c r="C8" s="2">
-        <v>62996</v>
+        <v>63185</v>
       </c>
       <c r="D8" t="s">
         <v>95</v>
@@ -1379,13 +1382,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C9" s="2">
-        <v>1852</v>
+        <v>2039</v>
       </c>
       <c r="D9" t="s">
         <v>95</v>
@@ -1396,13 +1399,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>34248</v>
+        <v>34255</v>
       </c>
       <c r="B10" s="2">
-        <v>192270</v>
+        <v>192320</v>
       </c>
       <c r="C10" s="2">
-        <v>1331352</v>
+        <v>1331670</v>
       </c>
       <c r="D10" t="s">
         <v>95</v>
@@ -1413,13 +1416,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>1326</v>
+        <v>1331</v>
       </c>
       <c r="B11" s="2">
-        <v>8426</v>
+        <v>8449</v>
       </c>
       <c r="C11" s="2">
-        <v>60797</v>
+        <v>60986</v>
       </c>
       <c r="D11" t="s">
         <v>95</v>
@@ -1430,13 +1433,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>1287</v>
+        <v>1292</v>
       </c>
       <c r="B12" s="2">
-        <v>8247</v>
+        <v>8270</v>
       </c>
       <c r="C12" s="2">
-        <v>59563</v>
+        <v>59752</v>
       </c>
       <c r="D12" t="s">
         <v>95</v>
@@ -1447,13 +1450,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="B13" s="2">
-        <v>2312</v>
+        <v>2342</v>
       </c>
       <c r="C13" s="2">
-        <v>17466</v>
+        <v>17676</v>
       </c>
       <c r="D13" t="s">
         <v>95</v>
@@ -1481,13 +1484,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>1365</v>
+        <v>1370</v>
       </c>
       <c r="B15" s="2">
-        <v>8565</v>
+        <v>8588</v>
       </c>
       <c r="C15" s="2">
-        <v>62005</v>
+        <v>62194</v>
       </c>
       <c r="D15" t="s">
         <v>95</v>
@@ -1498,13 +1501,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>1331</v>
+        <v>1336</v>
       </c>
       <c r="B16" s="2">
-        <v>8463</v>
+        <v>8486</v>
       </c>
       <c r="C16" s="2">
-        <v>61166</v>
+        <v>61355</v>
       </c>
       <c r="D16" t="s">
         <v>95</v>
@@ -1515,13 +1518,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>1375</v>
+        <v>1380</v>
       </c>
       <c r="B17" s="2">
-        <v>8662</v>
+        <v>8685</v>
       </c>
       <c r="C17" s="2">
-        <v>62750</v>
+        <v>62939</v>
       </c>
       <c r="D17" t="s">
         <v>95</v>
@@ -1532,13 +1535,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>1516</v>
+        <v>1522</v>
       </c>
       <c r="B18" s="2">
-        <v>6002</v>
+        <v>6032</v>
       </c>
       <c r="C18" s="2">
-        <v>40404</v>
+        <v>40615</v>
       </c>
       <c r="D18" t="s">
         <v>95</v>
@@ -1549,13 +1552,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>2580</v>
+        <v>2586</v>
       </c>
       <c r="B19" s="2">
-        <v>13599</v>
+        <v>13629</v>
       </c>
       <c r="C19" s="2">
-        <v>93582</v>
+        <v>93792</v>
       </c>
       <c r="D19" t="s">
         <v>95</v>
@@ -1566,13 +1569,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>1372</v>
+        <v>1377</v>
       </c>
       <c r="B20" s="2">
-        <v>8650</v>
+        <v>8673</v>
       </c>
       <c r="C20" s="2">
-        <v>62744</v>
+        <v>62933</v>
       </c>
       <c r="D20" t="s">
         <v>95</v>
@@ -1583,13 +1586,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>1575</v>
+        <v>1581</v>
       </c>
       <c r="B21" s="2">
-        <v>5552</v>
+        <v>5579</v>
       </c>
       <c r="C21" s="2">
-        <v>37856</v>
+        <v>38054</v>
       </c>
       <c r="D21" t="s">
         <v>95</v>
@@ -1600,13 +1603,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>33978</v>
+        <v>33984</v>
       </c>
       <c r="B22" s="2">
-        <v>177684</v>
+        <v>177719</v>
       </c>
       <c r="C22" s="2">
-        <v>1242179</v>
+        <v>1242418</v>
       </c>
       <c r="D22" t="s">
         <v>95</v>
@@ -1617,13 +1620,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="B23" s="2">
-        <v>1779</v>
+        <v>1803</v>
       </c>
       <c r="C23" s="2">
-        <v>13075</v>
+        <v>13268</v>
       </c>
       <c r="D23" t="s">
         <v>95</v>
@@ -1634,13 +1637,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B24" s="2">
-        <v>313</v>
+        <v>337</v>
       </c>
       <c r="C24" s="2">
-        <v>3238</v>
+        <v>3422</v>
       </c>
       <c r="D24" t="s">
         <v>95</v>
@@ -1651,13 +1654,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>1330</v>
+        <v>1335</v>
       </c>
       <c r="B25" s="2">
-        <v>8457</v>
+        <v>8480</v>
       </c>
       <c r="C25" s="2">
-        <v>61144</v>
+        <v>61333</v>
       </c>
       <c r="D25" t="s">
         <v>95</v>
@@ -1668,13 +1671,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>1328</v>
+        <v>1333</v>
       </c>
       <c r="B26" s="2">
-        <v>8413</v>
+        <v>8436</v>
       </c>
       <c r="C26" s="2">
-        <v>60871</v>
+        <v>61060</v>
       </c>
       <c r="D26" t="s">
         <v>95</v>
@@ -1685,13 +1688,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="B27" s="2">
-        <v>8127</v>
+        <v>8156</v>
       </c>
       <c r="C27" s="2">
-        <v>59927</v>
+        <v>60139</v>
       </c>
       <c r="D27" t="s">
         <v>95</v>
@@ -1702,13 +1705,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>1307</v>
+        <v>1312</v>
       </c>
       <c r="B28" s="2">
-        <v>8271</v>
+        <v>8294</v>
       </c>
       <c r="C28" s="2">
-        <v>59746</v>
+        <v>59935</v>
       </c>
       <c r="D28" t="s">
         <v>95</v>
@@ -1719,13 +1722,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>1377</v>
+        <v>1382</v>
       </c>
       <c r="B29" s="2">
-        <v>8624</v>
+        <v>8647</v>
       </c>
       <c r="C29" s="2">
-        <v>62647</v>
+        <v>62836</v>
       </c>
       <c r="D29" t="s">
         <v>95</v>
@@ -1736,13 +1739,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>1377</v>
+        <v>1382</v>
       </c>
       <c r="B30" s="2">
-        <v>8685</v>
+        <v>8708</v>
       </c>
       <c r="C30" s="2">
-        <v>62863</v>
+        <v>63052</v>
       </c>
       <c r="D30" t="s">
         <v>95</v>
@@ -1753,13 +1756,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>1313</v>
+        <v>1318</v>
       </c>
       <c r="B31" s="2">
-        <v>8293</v>
+        <v>8316</v>
       </c>
       <c r="C31" s="2">
-        <v>59969</v>
+        <v>60158</v>
       </c>
       <c r="D31" t="s">
         <v>95</v>
@@ -1770,13 +1773,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>1270</v>
+        <v>1275</v>
       </c>
       <c r="B32" s="2">
-        <v>8114</v>
+        <v>8137</v>
       </c>
       <c r="C32" s="2">
-        <v>58587</v>
+        <v>58776</v>
       </c>
       <c r="D32" t="s">
         <v>95</v>
@@ -1787,13 +1790,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>1284</v>
+        <v>1289</v>
       </c>
       <c r="B33" s="2">
-        <v>8239</v>
+        <v>8262</v>
       </c>
       <c r="C33" s="2">
-        <v>59453</v>
+        <v>59642</v>
       </c>
       <c r="D33" t="s">
         <v>95</v>
@@ -1804,13 +1807,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B34" s="2">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="C34" s="2">
-        <v>1883</v>
+        <v>2050</v>
       </c>
       <c r="D34" t="s">
         <v>96</v>
@@ -1821,13 +1824,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B35" s="2">
-        <v>1483</v>
+        <v>1522</v>
       </c>
       <c r="C35" s="2">
-        <v>9176</v>
+        <v>9451</v>
       </c>
       <c r="D35" t="s">
         <v>96</v>
@@ -1838,13 +1841,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>1332</v>
+        <v>1337</v>
       </c>
       <c r="B36" s="2">
-        <v>6900</v>
+        <v>6923</v>
       </c>
       <c r="C36" s="2">
-        <v>47130</v>
+        <v>47313</v>
       </c>
       <c r="D36" t="s">
         <v>96</v>
@@ -1872,13 +1875,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>53328</v>
+        <v>53340</v>
       </c>
       <c r="B38" s="2">
-        <v>289313</v>
+        <v>289377</v>
       </c>
       <c r="C38" s="2">
-        <v>2001832</v>
+        <v>2002369</v>
       </c>
       <c r="D38" t="s">
         <v>96</v>
@@ -1889,13 +1892,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="B39" s="2">
-        <v>1471</v>
+        <v>1494</v>
       </c>
       <c r="C39" s="2">
-        <v>11216</v>
+        <v>11400</v>
       </c>
       <c r="D39" t="s">
         <v>96</v>
@@ -1923,13 +1926,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B41" s="2">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="C41" s="2">
-        <v>2510</v>
+        <v>2674</v>
       </c>
       <c r="D41" t="s">
         <v>96</v>
@@ -1940,13 +1943,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>8926</v>
+        <v>8931</v>
       </c>
       <c r="B42" s="2">
-        <v>54412</v>
+        <v>54456</v>
       </c>
       <c r="C42" s="2">
-        <v>370446</v>
+        <v>370742</v>
       </c>
       <c r="D42" t="s">
         <v>96</v>
@@ -1957,13 +1960,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B43" s="2">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="C43" s="2">
-        <v>1726</v>
+        <v>1898</v>
       </c>
       <c r="D43" t="s">
         <v>97</v>
@@ -1974,13 +1977,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B44" s="2">
-        <v>396</v>
+        <v>435</v>
       </c>
       <c r="C44" s="2">
-        <v>3281</v>
+        <v>3552</v>
       </c>
       <c r="D44" t="s">
         <v>97</v>
@@ -2008,13 +2011,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>35201</v>
+        <v>35206</v>
       </c>
       <c r="B46" s="2">
-        <v>193899</v>
+        <v>193931</v>
       </c>
       <c r="C46" s="2">
-        <v>1346175</v>
+        <v>1346413</v>
       </c>
       <c r="D46" t="s">
         <v>97</v>
@@ -2025,13 +2028,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B47" s="2">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="C47" s="2">
-        <v>2141</v>
+        <v>2310</v>
       </c>
       <c r="D47" t="s">
         <v>97</v>
@@ -2042,13 +2045,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>2071</v>
+        <v>2075</v>
       </c>
       <c r="B48" s="2">
-        <v>10234</v>
+        <v>10252</v>
       </c>
       <c r="C48" s="2">
-        <v>69812</v>
+        <v>69979</v>
       </c>
       <c r="D48" t="s">
         <v>97</v>
@@ -2059,13 +2062,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>9880</v>
+        <v>9886</v>
       </c>
       <c r="B49" s="2">
-        <v>46772</v>
+        <v>46798</v>
       </c>
       <c r="C49" s="2">
-        <v>331789</v>
+        <v>331998</v>
       </c>
       <c r="D49" t="s">
         <v>98</v>
@@ -2076,13 +2079,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>128</v>
+        <v>264</v>
       </c>
       <c r="B50" s="2">
-        <v>311</v>
+        <v>1251</v>
       </c>
       <c r="C50" s="2">
-        <v>2296</v>
+        <v>10116</v>
       </c>
       <c r="D50" t="s">
         <v>98</v>
@@ -2093,13 +2096,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B51" s="2">
-        <v>363</v>
+        <v>380</v>
       </c>
       <c r="C51" s="2">
-        <v>2460</v>
+        <v>2618</v>
       </c>
       <c r="D51" t="s">
         <v>98</v>
@@ -2127,13 +2130,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>50734</v>
+        <v>50759</v>
       </c>
       <c r="B53" s="2">
-        <v>282946</v>
+        <v>283001</v>
       </c>
       <c r="C53" s="2">
-        <v>1980637</v>
+        <v>1981303</v>
       </c>
       <c r="D53" t="s">
         <v>98</v>
@@ -2161,1327 +2164,1344 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>53</v>
+        <v>691</v>
       </c>
       <c r="B55" s="2">
-        <v>205</v>
+        <v>3282</v>
       </c>
       <c r="C55" s="2">
-        <v>1690</v>
+        <v>25025</v>
       </c>
       <c r="D55" t="s">
         <v>98</v>
       </c>
       <c r="E55" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B56" s="2">
-        <v>1690</v>
+        <v>1705</v>
       </c>
       <c r="C56" s="2">
-        <v>15456</v>
+        <v>15615</v>
       </c>
       <c r="D56" t="s">
         <v>98</v>
       </c>
       <c r="E56" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>256</v>
+        <v>74</v>
       </c>
       <c r="B57" s="2">
-        <v>478</v>
+        <v>327</v>
       </c>
       <c r="C57" s="2">
-        <v>3190</v>
+        <v>2813</v>
       </c>
       <c r="D57" t="s">
         <v>98</v>
       </c>
       <c r="E57" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>1178</v>
+        <v>297</v>
       </c>
       <c r="B58" s="2">
-        <v>2001</v>
+        <v>667</v>
       </c>
       <c r="C58" s="2">
-        <v>12148</v>
+        <v>5095</v>
       </c>
       <c r="D58" t="s">
         <v>98</v>
       </c>
       <c r="E58" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>1678</v>
+        <v>1530</v>
       </c>
       <c r="B59" s="2">
-        <v>9473</v>
+        <v>4635</v>
       </c>
       <c r="C59" s="2">
-        <v>66161</v>
+        <v>33289</v>
       </c>
       <c r="D59" t="s">
         <v>98</v>
       </c>
       <c r="E59" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>9337</v>
+        <v>1703</v>
       </c>
       <c r="B60" s="2">
-        <v>43852</v>
+        <v>9537</v>
       </c>
       <c r="C60" s="2">
-        <v>311960</v>
+        <v>66629</v>
       </c>
       <c r="D60" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>77</v>
+        <v>9342</v>
       </c>
       <c r="B61" s="2">
-        <v>250</v>
+        <v>43876</v>
       </c>
       <c r="C61" s="2">
-        <v>1961</v>
+        <v>312154</v>
       </c>
       <c r="D61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E61" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>238</v>
+        <v>81</v>
       </c>
       <c r="B62" s="2">
-        <v>1004</v>
+        <v>267</v>
       </c>
       <c r="C62" s="2">
-        <v>7021</v>
+        <v>2115</v>
       </c>
       <c r="D62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E62" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>5</v>
+        <v>243</v>
       </c>
       <c r="B63" s="2">
-        <v>5</v>
+        <v>1037</v>
       </c>
       <c r="C63" s="2">
-        <v>97</v>
+        <v>7257</v>
       </c>
       <c r="D63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E63" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>42409</v>
+        <v>5</v>
       </c>
       <c r="B64" s="2">
-        <v>215859</v>
+        <v>5</v>
       </c>
       <c r="C64" s="2">
-        <v>1509074</v>
+        <v>97</v>
       </c>
       <c r="D64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E64" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>250</v>
+        <v>42449</v>
       </c>
       <c r="B65" s="2">
-        <v>1417</v>
+        <v>216014</v>
       </c>
       <c r="C65" s="2">
-        <v>9968</v>
+        <v>1510344</v>
       </c>
       <c r="D65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E65" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>129</v>
+        <v>250</v>
       </c>
       <c r="B66" s="2">
-        <v>363</v>
+        <v>1417</v>
       </c>
       <c r="C66" s="2">
-        <v>2991</v>
+        <v>9968</v>
       </c>
       <c r="D66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E66" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>245</v>
+        <v>133</v>
       </c>
       <c r="B67" s="2">
-        <v>887</v>
+        <v>377</v>
       </c>
       <c r="C67" s="2">
-        <v>6654</v>
+        <v>3139</v>
       </c>
       <c r="D67" t="s">
+        <v>103</v>
+      </c>
+      <c r="E67" t="s">
         <v>104</v>
-      </c>
-      <c r="E67" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>9675</v>
+        <v>255</v>
       </c>
       <c r="B68" s="2">
-        <v>46394</v>
+        <v>971</v>
       </c>
       <c r="C68" s="2">
-        <v>326938</v>
+        <v>7161</v>
       </c>
       <c r="D68" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E68" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>67</v>
+        <v>9680</v>
       </c>
       <c r="B69" s="2">
-        <v>217</v>
+        <v>46417</v>
       </c>
       <c r="C69" s="2">
-        <v>1701</v>
+        <v>327129</v>
       </c>
       <c r="D69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E69" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="B70" s="2">
-        <v>5</v>
+        <v>234</v>
       </c>
       <c r="C70" s="2">
-        <v>97</v>
+        <v>1857</v>
       </c>
       <c r="D70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E70" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>48343</v>
+        <v>5</v>
       </c>
       <c r="B71" s="2">
-        <v>270337</v>
+        <v>5</v>
       </c>
       <c r="C71" s="2">
-        <v>1870227</v>
+        <v>97</v>
       </c>
       <c r="D71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E71" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>47</v>
+        <v>48363</v>
       </c>
       <c r="B72" s="2">
-        <v>207</v>
+        <v>270417</v>
       </c>
       <c r="C72" s="2">
-        <v>1790</v>
+        <v>1870903</v>
       </c>
       <c r="D72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E72" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>1294</v>
+        <v>51</v>
       </c>
       <c r="B73" s="2">
-        <v>6908</v>
+        <v>224</v>
       </c>
       <c r="C73" s="2">
-        <v>47057</v>
+        <v>1943</v>
       </c>
       <c r="D73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E73" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>1616</v>
+        <v>1298</v>
       </c>
       <c r="B74" s="2">
-        <v>9750</v>
+        <v>6924</v>
       </c>
       <c r="C74" s="2">
-        <v>74727</v>
+        <v>47208</v>
       </c>
       <c r="D74" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E74" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>1556</v>
+        <v>1620</v>
       </c>
       <c r="B75" s="2">
-        <v>9289</v>
+        <v>9764</v>
       </c>
       <c r="C75" s="2">
-        <v>70778</v>
+        <v>74876</v>
       </c>
       <c r="D75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E75" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>1550</v>
+        <v>1560</v>
       </c>
       <c r="B76" s="2">
-        <v>9052</v>
+        <v>9303</v>
       </c>
       <c r="C76" s="2">
-        <v>69492</v>
+        <v>70927</v>
       </c>
       <c r="D76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E76" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>1434</v>
+        <v>1554</v>
       </c>
       <c r="B77" s="2">
-        <v>8658</v>
+        <v>9066</v>
       </c>
       <c r="C77" s="2">
-        <v>65742</v>
+        <v>69641</v>
       </c>
       <c r="D77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E77" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>1663</v>
+        <v>1438</v>
       </c>
       <c r="B78" s="2">
-        <v>10140</v>
+        <v>8672</v>
       </c>
       <c r="C78" s="2">
-        <v>77570</v>
+        <v>65891</v>
       </c>
       <c r="D78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E78" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>81</v>
+        <v>1667</v>
       </c>
       <c r="B79" s="2">
-        <v>286</v>
+        <v>10154</v>
       </c>
       <c r="C79" s="2">
-        <v>2055</v>
+        <v>77719</v>
       </c>
       <c r="D79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E79" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>37463</v>
+        <v>85</v>
       </c>
       <c r="B80" s="2">
-        <v>210805</v>
+        <v>301</v>
       </c>
       <c r="C80" s="2">
-        <v>1472010</v>
+        <v>2202</v>
       </c>
       <c r="D80" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E80" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>1405</v>
+        <v>37469</v>
       </c>
       <c r="B81" s="2">
-        <v>8705</v>
+        <v>210846</v>
       </c>
       <c r="C81" s="2">
-        <v>65698</v>
+        <v>1472288</v>
       </c>
       <c r="D81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E81" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>1795</v>
+        <v>1409</v>
       </c>
       <c r="B82" s="2">
-        <v>10304</v>
+        <v>8719</v>
       </c>
       <c r="C82" s="2">
-        <v>79450</v>
+        <v>65847</v>
       </c>
       <c r="D82" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E82" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>1594</v>
+        <v>1799</v>
       </c>
       <c r="B83" s="2">
-        <v>9491</v>
+        <v>10318</v>
       </c>
       <c r="C83" s="2">
-        <v>72691</v>
+        <v>79599</v>
       </c>
       <c r="D83" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E83" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="B84" s="2">
-        <v>9488</v>
+        <v>9505</v>
       </c>
       <c r="C84" s="2">
-        <v>72793</v>
+        <v>72840</v>
       </c>
       <c r="D84" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E84" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>4</v>
+        <v>1603</v>
       </c>
       <c r="B85" s="2">
-        <v>4</v>
+        <v>9502</v>
       </c>
       <c r="C85" s="2">
-        <v>67</v>
+        <v>72942</v>
       </c>
       <c r="D85" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E85" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>1482</v>
+        <v>4</v>
       </c>
       <c r="B86" s="2">
-        <v>9307</v>
+        <v>4</v>
       </c>
       <c r="C86" s="2">
-        <v>70292</v>
+        <v>67</v>
       </c>
       <c r="D86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E86" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>1647</v>
+        <v>1486</v>
       </c>
       <c r="B87" s="2">
-        <v>9645</v>
+        <v>9321</v>
       </c>
       <c r="C87" s="2">
-        <v>73867</v>
+        <v>70441</v>
       </c>
       <c r="D87" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E87" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>1698</v>
+        <v>1651</v>
       </c>
       <c r="B88" s="2">
-        <v>9822</v>
+        <v>9659</v>
       </c>
       <c r="C88" s="2">
-        <v>75574</v>
+        <v>74016</v>
       </c>
       <c r="D88" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E88" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>1692</v>
+        <v>1702</v>
       </c>
       <c r="B89" s="2">
-        <v>9781</v>
+        <v>9836</v>
       </c>
       <c r="C89" s="2">
-        <v>75053</v>
+        <v>75723</v>
       </c>
       <c r="D89" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E89" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>1551</v>
+        <v>1696</v>
       </c>
       <c r="B90" s="2">
-        <v>9063</v>
+        <v>9795</v>
       </c>
       <c r="C90" s="2">
-        <v>69588</v>
+        <v>75202</v>
       </c>
       <c r="D90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E90" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>1641</v>
+        <v>1555</v>
       </c>
       <c r="B91" s="2">
-        <v>9611</v>
+        <v>9077</v>
       </c>
       <c r="C91" s="2">
-        <v>73819</v>
+        <v>69737</v>
       </c>
       <c r="D91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E91" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>1709</v>
+        <v>1645</v>
       </c>
       <c r="B92" s="2">
-        <v>6065</v>
+        <v>9625</v>
       </c>
       <c r="C92" s="2">
-        <v>42181</v>
+        <v>73968</v>
       </c>
       <c r="D92" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E92" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>29486</v>
+        <v>1713</v>
       </c>
       <c r="B93" s="2">
-        <v>141273</v>
+        <v>6082</v>
       </c>
       <c r="C93" s="2">
-        <v>1011896</v>
+        <v>42337</v>
       </c>
       <c r="D93" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E93" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>38764</v>
+        <v>29490</v>
       </c>
       <c r="B94" s="2">
-        <v>204829</v>
+        <v>141291</v>
       </c>
       <c r="C94" s="2">
-        <v>1447381</v>
+        <v>1012065</v>
       </c>
       <c r="D94" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E94" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>4881</v>
+        <v>38769</v>
       </c>
       <c r="B95" s="2">
-        <v>27843</v>
+        <v>204855</v>
       </c>
       <c r="C95" s="2">
-        <v>198026</v>
+        <v>1447580</v>
       </c>
       <c r="D95" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E95" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>403</v>
+        <v>4887</v>
       </c>
       <c r="B96" s="2">
-        <v>1923</v>
+        <v>27882</v>
       </c>
       <c r="C96" s="2">
-        <v>14116</v>
+        <v>198293</v>
       </c>
       <c r="D96" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E96" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>71</v>
+        <v>407</v>
       </c>
       <c r="B97" s="2">
-        <v>355</v>
+        <v>1938</v>
       </c>
       <c r="C97" s="2">
-        <v>3350</v>
+        <v>14271</v>
       </c>
       <c r="D97" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E97" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>1508</v>
+        <v>75</v>
       </c>
       <c r="B98" s="2">
-        <v>9078</v>
+        <v>370</v>
       </c>
       <c r="C98" s="2">
-        <v>69144</v>
+        <v>3494</v>
       </c>
       <c r="D98" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E98" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>60191</v>
+        <v>1512</v>
       </c>
       <c r="B99" s="2">
-        <v>315018</v>
+        <v>9092</v>
       </c>
       <c r="C99" s="2">
-        <v>2217632</v>
+        <v>69293</v>
       </c>
       <c r="D99" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E99" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>1471</v>
+        <v>60197</v>
       </c>
       <c r="B100" s="2">
-        <v>8769</v>
+        <v>315054</v>
       </c>
       <c r="C100" s="2">
-        <v>66843</v>
+        <v>2217886</v>
       </c>
       <c r="D100" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E100" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>1588</v>
+        <v>1475</v>
       </c>
       <c r="B101" s="2">
-        <v>9343</v>
+        <v>8783</v>
       </c>
       <c r="C101" s="2">
-        <v>71684</v>
+        <v>66992</v>
       </c>
       <c r="D101" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E101" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>1636</v>
+        <v>1592</v>
       </c>
       <c r="B102" s="2">
-        <v>9577</v>
+        <v>9357</v>
       </c>
       <c r="C102" s="2">
-        <v>73309</v>
+        <v>71833</v>
       </c>
       <c r="D102" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E102" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>1725</v>
+        <v>1640</v>
       </c>
       <c r="B103" s="2">
-        <v>10027</v>
+        <v>9591</v>
       </c>
       <c r="C103" s="2">
-        <v>77080</v>
+        <v>73458</v>
       </c>
       <c r="D103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E103" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>3375</v>
+        <v>1729</v>
       </c>
       <c r="B104" s="2">
-        <v>17590</v>
+        <v>10041</v>
       </c>
       <c r="C104" s="2">
-        <v>125028</v>
+        <v>77229</v>
       </c>
       <c r="D104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E104" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>1574</v>
+        <v>3379</v>
       </c>
       <c r="B105" s="2">
-        <v>9407</v>
+        <v>17604</v>
       </c>
       <c r="C105" s="2">
-        <v>72067</v>
+        <v>125170</v>
       </c>
       <c r="D105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E105" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>1559</v>
+        <v>1578</v>
       </c>
       <c r="B106" s="2">
-        <v>9474</v>
+        <v>9421</v>
       </c>
       <c r="C106" s="2">
-        <v>72099</v>
+        <v>72216</v>
       </c>
       <c r="D106" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E106" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>1481</v>
+        <v>1563</v>
       </c>
       <c r="B107" s="2">
-        <v>8960</v>
+        <v>9488</v>
       </c>
       <c r="C107" s="2">
-        <v>68123</v>
+        <v>72248</v>
       </c>
       <c r="D107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E107" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>4</v>
+        <v>1485</v>
       </c>
       <c r="B108" s="2">
-        <v>4</v>
+        <v>8974</v>
       </c>
       <c r="C108" s="2">
-        <v>73</v>
+        <v>68272</v>
       </c>
       <c r="D108" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E108" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>20106</v>
+        <v>4</v>
       </c>
       <c r="B109" s="2">
-        <v>113443</v>
+        <v>4</v>
       </c>
       <c r="C109" s="2">
-        <v>795564</v>
+        <v>73</v>
       </c>
       <c r="D109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E109" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>15370</v>
+        <v>20114</v>
       </c>
       <c r="B110" s="2">
-        <v>85461</v>
+        <v>113474</v>
       </c>
       <c r="C110" s="2">
-        <v>596981</v>
+        <v>795861</v>
       </c>
       <c r="D110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E110" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>3450</v>
+        <v>15374</v>
       </c>
       <c r="B111" s="2">
-        <v>23659</v>
+        <v>85480</v>
       </c>
       <c r="C111" s="2">
-        <v>140126</v>
+        <v>597137</v>
       </c>
       <c r="D111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E111" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>2815</v>
+        <v>3454</v>
       </c>
       <c r="B112" s="2">
-        <v>21242</v>
+        <v>23678</v>
       </c>
       <c r="C112" s="2">
-        <v>117692</v>
+        <v>140282</v>
       </c>
       <c r="D112" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E112" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>14652</v>
+        <v>2819</v>
       </c>
       <c r="B113" s="2">
-        <v>90343</v>
+        <v>21261</v>
       </c>
       <c r="C113" s="2">
-        <v>624013</v>
+        <v>117848</v>
       </c>
       <c r="D113" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E113" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>24508</v>
+        <v>14656</v>
       </c>
       <c r="B114" s="2">
-        <v>142110</v>
+        <v>90362</v>
       </c>
       <c r="C114" s="2">
-        <v>982692</v>
+        <v>624169</v>
       </c>
       <c r="D114" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E114" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>18705</v>
+        <v>24512</v>
       </c>
       <c r="B115" s="2">
-        <v>70113</v>
+        <v>142129</v>
       </c>
       <c r="C115" s="2">
-        <v>506556</v>
+        <v>982848</v>
       </c>
       <c r="D115" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E115" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>7795</v>
+        <v>18709</v>
       </c>
       <c r="B116" s="2">
-        <v>47700</v>
+        <v>70132</v>
       </c>
       <c r="C116" s="2">
-        <v>310256</v>
+        <v>506712</v>
       </c>
       <c r="D116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E116" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>6462</v>
+        <v>7799</v>
       </c>
       <c r="B117" s="2">
-        <v>27658</v>
+        <v>47719</v>
       </c>
       <c r="C117" s="2">
-        <v>214828</v>
+        <v>310412</v>
       </c>
       <c r="D117" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E117" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>83</v>
+        <v>6462</v>
       </c>
       <c r="B118" s="2">
-        <v>351</v>
+        <v>27662</v>
       </c>
       <c r="C118" s="2">
-        <v>2830</v>
+        <v>214845</v>
       </c>
       <c r="D118" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E118" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>43729</v>
+        <v>87</v>
       </c>
       <c r="B119" s="2">
-        <v>226939</v>
+        <v>366</v>
       </c>
       <c r="C119" s="2">
-        <v>1676643</v>
+        <v>2974</v>
       </c>
       <c r="D119" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E119" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>4057</v>
+        <v>43729</v>
       </c>
       <c r="B120" s="2">
-        <v>23760</v>
+        <v>226939</v>
       </c>
       <c r="C120" s="2">
-        <v>177234</v>
+        <v>1676643</v>
       </c>
       <c r="D120" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E120" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>4252</v>
+        <v>4057</v>
       </c>
       <c r="B121" s="2">
-        <v>23482</v>
+        <v>23760</v>
       </c>
       <c r="C121" s="2">
-        <v>182662</v>
+        <v>177234</v>
       </c>
       <c r="D121" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E121" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>2839</v>
+        <v>4252</v>
       </c>
       <c r="B122" s="2">
-        <v>21250</v>
+        <v>23482</v>
       </c>
       <c r="C122" s="2">
-        <v>141291</v>
+        <v>182662</v>
       </c>
       <c r="D122" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E122" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>4143</v>
+        <v>2839</v>
       </c>
       <c r="B123" s="2">
-        <v>23702</v>
+        <v>21250</v>
       </c>
       <c r="C123" s="2">
-        <v>176613</v>
+        <v>141291</v>
       </c>
       <c r="D123" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E123" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>4048</v>
+        <v>4143</v>
       </c>
       <c r="B124" s="2">
-        <v>23552</v>
+        <v>23702</v>
       </c>
       <c r="C124" s="2">
-        <v>175100</v>
+        <v>176613</v>
       </c>
       <c r="D124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E124" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>83</v>
+        <v>4048</v>
       </c>
       <c r="B125" s="2">
-        <v>338</v>
+        <v>23552</v>
       </c>
       <c r="C125" s="2">
-        <v>3765</v>
+        <v>175100</v>
       </c>
       <c r="D125" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E125" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>4184</v>
+        <v>83</v>
       </c>
       <c r="B126" s="2">
-        <v>24090</v>
+        <v>338</v>
       </c>
       <c r="C126" s="2">
-        <v>179462</v>
+        <v>3765</v>
       </c>
       <c r="D126" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E126" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>274</v>
+        <v>4184</v>
       </c>
       <c r="B127" s="2">
-        <v>1736</v>
+        <v>24090</v>
       </c>
       <c r="C127" s="2">
-        <v>10228</v>
+        <v>179462</v>
       </c>
       <c r="D127" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E127" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>1</v>
+        <v>274</v>
       </c>
       <c r="B128" s="2">
-        <v>1</v>
+        <v>1736</v>
       </c>
       <c r="C128" s="2">
-        <v>11</v>
+        <v>10228</v>
       </c>
       <c r="D128" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E128" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B129" s="2">
-        <v>159</v>
+        <v>1</v>
       </c>
       <c r="C129" s="2">
-        <v>1432</v>
+        <v>11</v>
       </c>
       <c r="D129" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E129" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>31403</v>
+        <v>34</v>
       </c>
       <c r="B130" s="2">
-        <v>178050</v>
+        <v>159</v>
       </c>
       <c r="C130" s="2">
-        <v>1248094</v>
+        <v>1432</v>
       </c>
       <c r="D130" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E130" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>15079</v>
+        <v>31403</v>
       </c>
       <c r="B131" s="2">
-        <v>83051</v>
+        <v>178050</v>
       </c>
       <c r="C131" s="2">
-        <v>720970</v>
+        <v>1248094</v>
       </c>
       <c r="D131" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E131" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
+        <v>15079</v>
+      </c>
+      <c r="B132" s="2">
+        <v>83051</v>
+      </c>
+      <c r="C132" s="2">
+        <v>720970</v>
+      </c>
+      <c r="D132" t="s">
+        <v>111</v>
+      </c>
+      <c r="E132" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="2">
         <v>173</v>
       </c>
-      <c r="B132" s="2">
+      <c r="B133" s="2">
         <v>608</v>
       </c>
-      <c r="C132" s="2">
+      <c r="C133" s="2">
         <v>5900</v>
       </c>
-      <c r="D132" t="s">
-        <v>112</v>
-      </c>
-      <c r="E132" t="s">
+      <c r="D133" t="s">
+        <v>111</v>
+      </c>
+      <c r="E133" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3495,10 +3515,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3810105-F70C-6549-8E2A-9ACB8CFD3E2D}">
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:C133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C133"/>
+      <selection sqref="A1:C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3510,7 +3530,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
         <v>94</v>
@@ -3521,7 +3541,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>653</v>
+        <v>684</v>
       </c>
       <c r="B2" t="s">
         <v>94</v>
@@ -3543,7 +3563,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>156986</v>
+        <v>157013</v>
       </c>
       <c r="B4" t="s">
         <v>94</v>
@@ -3554,7 +3574,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>94</v>
@@ -3565,7 +3585,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>13530</v>
+        <v>13545</v>
       </c>
       <c r="B6" t="s">
         <v>94</v>
@@ -3576,7 +3596,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>3207</v>
+        <v>3221</v>
       </c>
       <c r="B7" t="s">
         <v>95</v>
@@ -3587,7 +3607,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>3398</v>
+        <v>3412</v>
       </c>
       <c r="B8" t="s">
         <v>95</v>
@@ -3598,7 +3618,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
         <v>95</v>
@@ -3609,7 +3629,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>147257</v>
+        <v>147303</v>
       </c>
       <c r="B10" t="s">
         <v>95</v>
@@ -3620,7 +3640,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>3206</v>
+        <v>3220</v>
       </c>
       <c r="B11" t="s">
         <v>95</v>
@@ -3631,7 +3651,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>3061</v>
+        <v>3075</v>
       </c>
       <c r="B12" t="s">
         <v>95</v>
@@ -3642,7 +3662,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>1632</v>
+        <v>1655</v>
       </c>
       <c r="B13" t="s">
         <v>95</v>
@@ -3664,7 +3684,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>3368</v>
+        <v>3382</v>
       </c>
       <c r="B15" t="s">
         <v>95</v>
@@ -3675,7 +3695,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>3215</v>
+        <v>3229</v>
       </c>
       <c r="B16" t="s">
         <v>95</v>
@@ -3686,7 +3706,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>3364</v>
+        <v>3378</v>
       </c>
       <c r="B17" t="s">
         <v>95</v>
@@ -3697,7 +3717,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>3295</v>
+        <v>3318</v>
       </c>
       <c r="B18" t="s">
         <v>95</v>
@@ -3708,7 +3728,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>9655</v>
+        <v>9678</v>
       </c>
       <c r="B19" t="s">
         <v>95</v>
@@ -3719,7 +3739,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>3396</v>
+        <v>3410</v>
       </c>
       <c r="B20" t="s">
         <v>95</v>
@@ -3730,7 +3750,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>2045</v>
+        <v>2064</v>
       </c>
       <c r="B21" t="s">
         <v>95</v>
@@ -3741,7 +3761,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>125439</v>
+        <v>125471</v>
       </c>
       <c r="B22" t="s">
         <v>95</v>
@@ -3752,7 +3772,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>816</v>
+        <v>832</v>
       </c>
       <c r="B23" t="s">
         <v>95</v>
@@ -3763,7 +3783,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
         <v>95</v>
@@ -3774,7 +3794,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>3225</v>
+        <v>3239</v>
       </c>
       <c r="B25" t="s">
         <v>95</v>
@@ -3785,7 +3805,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>3225</v>
+        <v>3239</v>
       </c>
       <c r="B26" t="s">
         <v>95</v>
@@ -3796,7 +3816,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>6114</v>
+        <v>6134</v>
       </c>
       <c r="B27" t="s">
         <v>95</v>
@@ -3807,7 +3827,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>3183</v>
+        <v>3197</v>
       </c>
       <c r="B28" t="s">
         <v>95</v>
@@ -3818,7 +3838,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>3376</v>
+        <v>3390</v>
       </c>
       <c r="B29" t="s">
         <v>95</v>
@@ -3829,7 +3849,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>3396</v>
+        <v>3410</v>
       </c>
       <c r="B30" t="s">
         <v>95</v>
@@ -3840,7 +3860,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>3202</v>
+        <v>3216</v>
       </c>
       <c r="B31" t="s">
         <v>95</v>
@@ -3851,7 +3871,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>3036</v>
+        <v>3050</v>
       </c>
       <c r="B32" t="s">
         <v>95</v>
@@ -3862,7 +3882,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>3063</v>
+        <v>3077</v>
       </c>
       <c r="B33" t="s">
         <v>95</v>
@@ -3873,7 +3893,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
         <v>96</v>
@@ -3884,7 +3904,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>297</v>
+        <v>329</v>
       </c>
       <c r="B35" t="s">
         <v>96</v>
@@ -3895,7 +3915,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>5040</v>
+        <v>5057</v>
       </c>
       <c r="B36" t="s">
         <v>96</v>
@@ -3917,7 +3937,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>196232</v>
+        <v>196285</v>
       </c>
       <c r="B38" t="s">
         <v>96</v>
@@ -3928,7 +3948,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>1053</v>
+        <v>1070</v>
       </c>
       <c r="B39" t="s">
         <v>96</v>
@@ -3950,7 +3970,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B41" t="s">
         <v>96</v>
@@ -3961,7 +3981,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>42194</v>
+        <v>42232</v>
       </c>
       <c r="B42" t="s">
         <v>96</v>
@@ -3972,7 +3992,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
         <v>97</v>
@@ -3983,7 +4003,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
@@ -4005,7 +4025,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>142605</v>
+        <v>142629</v>
       </c>
       <c r="B46" t="s">
         <v>97</v>
@@ -4016,7 +4036,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B47" t="s">
         <v>97</v>
@@ -4027,7 +4047,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>7404</v>
+        <v>7416</v>
       </c>
       <c r="B48" t="s">
         <v>97</v>
@@ -4038,7 +4058,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>16282</v>
+        <v>16301</v>
       </c>
       <c r="B49" t="s">
         <v>98</v>
@@ -4049,7 +4069,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>113</v>
+        <v>877</v>
       </c>
       <c r="B50" t="s">
         <v>98</v>
@@ -4060,7 +4080,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
         <v>98</v>
@@ -4082,7 +4102,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>215227</v>
+        <v>215260</v>
       </c>
       <c r="B53" t="s">
         <v>98</v>
@@ -4104,859 +4124,870 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>109</v>
+        <v>2304</v>
       </c>
       <c r="B55" t="s">
         <v>98</v>
       </c>
       <c r="C55" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>777</v>
+        <v>787</v>
       </c>
       <c r="B56" t="s">
         <v>98</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>109</v>
+        <v>202</v>
       </c>
       <c r="B57" t="s">
         <v>98</v>
       </c>
       <c r="C57" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B58" t="s">
         <v>98</v>
       </c>
       <c r="C58" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>6008</v>
+        <v>2581</v>
       </c>
       <c r="B59" t="s">
         <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>15401</v>
+        <v>6050</v>
       </c>
       <c r="B60" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>105</v>
+        <v>15419</v>
       </c>
       <c r="B61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C61" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>274</v>
+        <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>0</v>
+        <v>301</v>
       </c>
       <c r="B63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>160312</v>
+        <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>1082</v>
+        <v>160424</v>
       </c>
       <c r="B65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>180</v>
+        <v>1082</v>
       </c>
       <c r="B66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C66" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>255</v>
+        <v>189</v>
       </c>
       <c r="B67" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" t="s">
         <v>104</v>
-      </c>
-      <c r="C67" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>16087</v>
+        <v>328</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>92</v>
+        <v>16105</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C69" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>205318</v>
+        <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C71" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>116</v>
+        <v>205378</v>
       </c>
       <c r="B72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C72" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>5149</v>
+        <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C73" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>4481</v>
+        <v>5159</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C74" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>3915</v>
+        <v>4489</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C75" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>3882</v>
+        <v>3923</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C76" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>3593</v>
+        <v>3890</v>
       </c>
       <c r="B77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C77" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>4869</v>
+        <v>3601</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C78" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>133</v>
+        <v>4877</v>
       </c>
       <c r="B79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C79" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>163635</v>
+        <v>142</v>
       </c>
       <c r="B80" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C80" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>3510</v>
+        <v>163672</v>
       </c>
       <c r="B81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C81" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>4821</v>
+        <v>3518</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C82" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>4194</v>
+        <v>4829</v>
       </c>
       <c r="B83" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C83" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>4229</v>
+        <v>4202</v>
       </c>
       <c r="B84" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C84" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>0</v>
+        <v>4237</v>
       </c>
       <c r="B85" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C85" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>4131</v>
+        <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C86" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>4229</v>
+        <v>4139</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C87" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>4574</v>
+        <v>4237</v>
       </c>
       <c r="B88" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C88" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>4331</v>
+        <v>4582</v>
       </c>
       <c r="B89" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C89" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>3887</v>
+        <v>4339</v>
       </c>
       <c r="B90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>4161</v>
+        <v>3895</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C91" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>2402</v>
+        <v>4169</v>
       </c>
       <c r="B92" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C92" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>95374</v>
+        <v>2415</v>
       </c>
       <c r="B93" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C93" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>148740</v>
+        <v>95390</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C94" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>21674</v>
+        <v>148763</v>
       </c>
       <c r="B95" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C95" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>952</v>
+        <v>21706</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C96" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>159</v>
+        <v>962</v>
       </c>
       <c r="B97" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C97" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>3777</v>
+        <v>169</v>
       </c>
       <c r="B98" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C98" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>210399</v>
+        <v>3785</v>
       </c>
       <c r="B99" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C99" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>3693</v>
+        <v>210428</v>
       </c>
       <c r="B100" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C100" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>3995</v>
+        <v>3701</v>
       </c>
       <c r="B101" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C101" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>4163</v>
+        <v>4003</v>
       </c>
       <c r="B102" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C102" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>4625</v>
+        <v>4171</v>
       </c>
       <c r="B103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C103" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>13261</v>
+        <v>4633</v>
       </c>
       <c r="B104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C104" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>4135</v>
+        <v>13269</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>4175</v>
+        <v>4143</v>
       </c>
       <c r="B106" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C106" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>3718</v>
+        <v>4183</v>
       </c>
       <c r="B107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C107" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>0</v>
+        <v>3726</v>
       </c>
       <c r="B108" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C108" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>85033</v>
+        <v>0</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C109" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>60287</v>
+        <v>85055</v>
       </c>
       <c r="B110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C110" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>5355</v>
+        <v>60301</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C111" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>2214</v>
+        <v>5369</v>
       </c>
       <c r="B112" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C112" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>60087</v>
+        <v>2228</v>
       </c>
       <c r="B113" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C113" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>109530</v>
+        <v>60101</v>
       </c>
       <c r="B114" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C114" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>31189</v>
+        <v>109544</v>
       </c>
       <c r="B115" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C115" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>26105</v>
+        <v>31203</v>
       </c>
       <c r="B116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C116" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>19917</v>
+        <v>26119</v>
       </c>
       <c r="B117" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C117" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>228</v>
+        <v>19921</v>
       </c>
       <c r="B118" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C118" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>170098</v>
+        <v>238</v>
       </c>
       <c r="B119" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C119" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>16949</v>
+        <v>170098</v>
       </c>
       <c r="B120" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C120" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>16602</v>
+        <v>16949</v>
       </c>
       <c r="B121" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C121" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>14995</v>
+        <v>16602</v>
       </c>
       <c r="B122" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C122" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>16974</v>
+        <v>14995</v>
       </c>
       <c r="B123" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C123" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>16789</v>
+        <v>16974</v>
       </c>
       <c r="B124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C124" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>106</v>
+        <v>16789</v>
       </c>
       <c r="B125" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C125" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>17257</v>
+        <v>106</v>
       </c>
       <c r="B126" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C126" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>117</v>
+        <v>17257</v>
       </c>
       <c r="B127" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C127" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="B128" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C128" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="B129" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C129" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>133362</v>
+        <v>95</v>
       </c>
       <c r="B130" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C130" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>52571</v>
+        <v>133362</v>
       </c>
       <c r="B131" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C131" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
+        <v>52571</v>
+      </c>
+      <c r="B132" t="s">
+        <v>111</v>
+      </c>
+      <c r="C132" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="2">
         <v>390</v>
       </c>
-      <c r="B132" t="s">
-        <v>112</v>
-      </c>
-      <c r="C132" t="s">
+      <c r="B133" t="s">
+        <v>111</v>
+      </c>
+      <c r="C133" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Commodore 64 section
</commit_message>
<xml_diff>
--- a/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
+++ b/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mark/Documents/Files/Websites/Repositories/bbcelite-scripts/code-analysis/word-count-code-comments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B80DC9-781B-334E-8999-B01BA49E7B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B8C648-B088-8A4C-8A6D-64BFF061FDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12060" yWindow="2180" windowWidth="21600" windowHeight="17440" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
+    <workbookView xWindow="17280" yWindow="2800" windowWidth="21600" windowHeight="17440" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="3" r:id="rId1"/>
@@ -833,11 +833,11 @@
       </c>
       <c r="C3" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A3)</f>
-        <v>400079</v>
+        <v>400080</v>
       </c>
       <c r="D3" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A3)</f>
-        <v>622267</v>
+        <v>622268</v>
       </c>
       <c r="H3" t="s">
         <v>83</v>
@@ -895,15 +895,15 @@
       </c>
       <c r="B6" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A6,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>65989</v>
+        <v>65956</v>
       </c>
       <c r="C6" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A6)</f>
-        <v>246255</v>
+        <v>246338</v>
       </c>
       <c r="D6" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A6)</f>
-        <v>353566</v>
+        <v>353634</v>
       </c>
       <c r="H6" t="s">
         <v>82</v>
@@ -967,15 +967,15 @@
       </c>
       <c r="B9" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A9,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>59341</v>
+        <v>59427</v>
       </c>
       <c r="C9" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A9)</f>
-        <v>226873</v>
+        <v>227487</v>
       </c>
       <c r="D9" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A9)</f>
-        <v>324221</v>
+        <v>324958</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -985,15 +985,15 @@
       </c>
       <c r="B10" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A10,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>52672</v>
+        <v>52696</v>
       </c>
       <c r="C10" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A10)</f>
-        <v>177860</v>
+        <v>177957</v>
       </c>
       <c r="D10" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A10)</f>
-        <v>263964</v>
+        <v>264089</v>
       </c>
       <c r="H10" t="s">
         <v>84</v>
@@ -1085,15 +1085,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5">
         <f>SUM(B2:B14)</f>
-        <v>867249</v>
+        <v>867326</v>
       </c>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>3175957</v>
+        <v>3176752</v>
       </c>
       <c r="D15" s="5">
         <f>SUM(D2:D14)</f>
-        <v>4674039</v>
+        <v>4674970</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1881,7 +1881,7 @@
         <v>289377</v>
       </c>
       <c r="C38" s="2">
-        <v>2002369</v>
+        <v>2002363</v>
       </c>
       <c r="D38" t="s">
         <v>96</v>
@@ -2085,7 +2085,7 @@
         <v>1251</v>
       </c>
       <c r="C50" s="2">
-        <v>10116</v>
+        <v>10107</v>
       </c>
       <c r="D50" t="s">
         <v>98</v>
@@ -2130,13 +2130,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>50759</v>
+        <v>50776</v>
       </c>
       <c r="B53" s="2">
-        <v>283001</v>
+        <v>283174</v>
       </c>
       <c r="C53" s="2">
-        <v>1981303</v>
+        <v>1982569</v>
       </c>
       <c r="D53" t="s">
         <v>98</v>
@@ -2201,10 +2201,10 @@
         <v>74</v>
       </c>
       <c r="B57" s="2">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C57" s="2">
-        <v>2813</v>
+        <v>2791</v>
       </c>
       <c r="D57" t="s">
         <v>98</v>
@@ -2218,10 +2218,10 @@
         <v>297</v>
       </c>
       <c r="B58" s="2">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C58" s="2">
-        <v>5095</v>
+        <v>5092</v>
       </c>
       <c r="D58" t="s">
         <v>98</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>1530</v>
+        <v>1536</v>
       </c>
       <c r="B59" s="2">
-        <v>4635</v>
+        <v>4655</v>
       </c>
       <c r="C59" s="2">
-        <v>33289</v>
+        <v>33475</v>
       </c>
       <c r="D59" t="s">
         <v>98</v>
@@ -2249,13 +2249,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>1703</v>
+        <v>1647</v>
       </c>
       <c r="B60" s="2">
-        <v>9537</v>
+        <v>9421</v>
       </c>
       <c r="C60" s="2">
-        <v>66629</v>
+        <v>65662</v>
       </c>
       <c r="D60" t="s">
         <v>98</v>
@@ -2334,13 +2334,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>42449</v>
+        <v>42473</v>
       </c>
       <c r="B65" s="2">
-        <v>216014</v>
+        <v>216139</v>
       </c>
       <c r="C65" s="2">
-        <v>1510344</v>
+        <v>1511272</v>
       </c>
       <c r="D65" t="s">
         <v>103</v>
@@ -2402,13 +2402,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>9680</v>
+        <v>9688</v>
       </c>
       <c r="B69" s="2">
-        <v>46417</v>
+        <v>46430</v>
       </c>
       <c r="C69" s="2">
-        <v>327129</v>
+        <v>327338</v>
       </c>
       <c r="D69" t="s">
         <v>106</v>
@@ -2453,13 +2453,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>48363</v>
+        <v>48441</v>
       </c>
       <c r="B72" s="2">
-        <v>270417</v>
+        <v>271141</v>
       </c>
       <c r="C72" s="2">
-        <v>1870903</v>
+        <v>1875698</v>
       </c>
       <c r="D72" t="s">
         <v>106</v>
@@ -3139,7 +3139,7 @@
         <v>23678</v>
       </c>
       <c r="C112" s="2">
-        <v>140282</v>
+        <v>140274</v>
       </c>
       <c r="D112" t="s">
         <v>108</v>
@@ -3238,10 +3238,10 @@
         <v>6462</v>
       </c>
       <c r="B118" s="2">
-        <v>27662</v>
+        <v>27663</v>
       </c>
       <c r="C118" s="2">
-        <v>214845</v>
+        <v>214850</v>
       </c>
       <c r="D118" t="s">
         <v>108</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>215260</v>
+        <v>215405</v>
       </c>
       <c r="B53" t="s">
         <v>98</v>
@@ -4146,7 +4146,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B57" t="s">
         <v>98</v>
@@ -4157,7 +4157,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B58" t="s">
         <v>98</v>
@@ -4168,7 +4168,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>2581</v>
+        <v>2594</v>
       </c>
       <c r="B59" t="s">
         <v>98</v>
@@ -4179,7 +4179,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>6050</v>
+        <v>5984</v>
       </c>
       <c r="B60" t="s">
         <v>98</v>
@@ -4234,7 +4234,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>160424</v>
+        <v>160521</v>
       </c>
       <c r="B65" t="s">
         <v>103</v>
@@ -4311,7 +4311,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>205378</v>
+        <v>205992</v>
       </c>
       <c r="B72" t="s">
         <v>106</v>
@@ -4817,7 +4817,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>19921</v>
+        <v>19922</v>
       </c>
       <c r="B118" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
Update image and spelling scripts with finished Apple II version
</commit_message>
<xml_diff>
--- a/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
+++ b/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mark/Documents/Files/Websites/Repositories/bbcelite-scripts/code-analysis/word-count-code-comments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B8C648-B088-8A4C-8A6D-64BFF061FDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D9828A-FB4A-7244-A737-0BE0C25932F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="2800" windowWidth="21600" windowHeight="17440" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
   </bookViews>
@@ -773,7 +773,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4742C6F-ED5A-B74D-BFAE-09A904247301}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -805,15 +807,15 @@
       </c>
       <c r="B2" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A2,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$I$4</f>
-        <v>151582</v>
+        <v>151399</v>
       </c>
       <c r="C2" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A2)</f>
-        <v>520054</v>
+        <v>517784</v>
       </c>
       <c r="D2" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A2)</f>
-        <v>800354</v>
+        <v>797920</v>
       </c>
       <c r="H2" t="s">
         <v>81</v>
@@ -829,15 +831,15 @@
       </c>
       <c r="B3" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A3,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>113986</v>
+        <v>113991</v>
       </c>
       <c r="C3" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A3)</f>
-        <v>400080</v>
+        <v>399859</v>
       </c>
       <c r="D3" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A3)</f>
-        <v>622268</v>
+        <v>622074</v>
       </c>
       <c r="H3" t="s">
         <v>83</v>
@@ -853,15 +855,15 @@
       </c>
       <c r="B4" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A4,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$I$8</f>
-        <v>100795</v>
+        <v>100863</v>
       </c>
       <c r="C4" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A4)</f>
-        <v>348837</v>
+        <v>347923</v>
       </c>
       <c r="D4" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A4)</f>
-        <v>543750</v>
+        <v>542914</v>
       </c>
       <c r="H4" t="s">
         <v>86</v>
@@ -895,15 +897,15 @@
       </c>
       <c r="B6" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A6,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>65956</v>
+        <v>66076</v>
       </c>
       <c r="C6" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A6)</f>
-        <v>246338</v>
+        <v>246802</v>
       </c>
       <c r="D6" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A6)</f>
-        <v>353634</v>
+        <v>354231</v>
       </c>
       <c r="H6" t="s">
         <v>82</v>
@@ -919,15 +921,15 @@
       </c>
       <c r="B7" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A7,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>65084</v>
+        <v>65063</v>
       </c>
       <c r="C7" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A7)</f>
-        <v>232134</v>
+        <v>231708</v>
       </c>
       <c r="D7" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A7)</f>
-        <v>342936</v>
+        <v>342496</v>
       </c>
       <c r="H7" t="s">
         <v>85</v>
@@ -943,15 +945,15 @@
       </c>
       <c r="B8" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A8,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>64419</v>
+        <v>64459</v>
       </c>
       <c r="C8" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A8)</f>
-        <v>245575</v>
+        <v>245261</v>
       </c>
       <c r="D8" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A8)</f>
-        <v>354905</v>
+        <v>354652</v>
       </c>
       <c r="H8" t="s">
         <v>86</v>
@@ -967,15 +969,15 @@
       </c>
       <c r="B9" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A9,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>59427</v>
+        <v>59500</v>
       </c>
       <c r="C9" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A9)</f>
-        <v>227487</v>
+        <v>227458</v>
       </c>
       <c r="D9" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A9)</f>
-        <v>324958</v>
+        <v>325019</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -985,15 +987,15 @@
       </c>
       <c r="B10" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A10,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>52696</v>
+        <v>57337</v>
       </c>
       <c r="C10" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A10)</f>
-        <v>177957</v>
+        <v>216442</v>
       </c>
       <c r="D10" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A10)</f>
-        <v>264089</v>
+        <v>308402</v>
       </c>
       <c r="H10" t="s">
         <v>84</v>
@@ -1006,15 +1008,15 @@
       </c>
       <c r="B11" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A11,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>41776</v>
+        <v>41752</v>
       </c>
       <c r="C11" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A11)</f>
-        <v>171489</v>
+        <v>170988</v>
       </c>
       <c r="D11" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A11)</f>
-        <v>232255</v>
+        <v>231741</v>
       </c>
       <c r="H11" t="s">
         <v>2</v>
@@ -1030,15 +1032,15 @@
       </c>
       <c r="B12" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A12,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>37424</v>
+        <v>37365</v>
       </c>
       <c r="C12" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A12)</f>
-        <v>150496</v>
+        <v>149984</v>
       </c>
       <c r="D12" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A12)</f>
-        <v>205103</v>
+        <v>204534</v>
       </c>
       <c r="H12" t="s">
         <v>8</v>
@@ -1085,15 +1087,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5">
         <f>SUM(B2:B14)</f>
-        <v>867326</v>
+        <v>871986</v>
       </c>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>3176752</v>
+        <v>3210514</v>
       </c>
       <c r="D15" s="5">
         <f>SUM(D2:D14)</f>
-        <v>4674970</v>
+        <v>4714701</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1297,13 +1299,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>38158</v>
+        <v>38133</v>
       </c>
       <c r="B4" s="2">
-        <v>212605</v>
+        <v>212138</v>
       </c>
       <c r="C4" s="2">
-        <v>1475037</v>
+        <v>1472417</v>
       </c>
       <c r="D4" t="s">
         <v>94</v>
@@ -1331,13 +1333,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>3367</v>
+        <v>3368</v>
       </c>
       <c r="B6" s="2">
-        <v>18088</v>
+        <v>18041</v>
       </c>
       <c r="C6" s="2">
-        <v>125040</v>
+        <v>124732</v>
       </c>
       <c r="D6" t="s">
         <v>94</v>
@@ -1348,13 +1350,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>1328</v>
+        <v>1335</v>
       </c>
       <c r="B7" s="2">
-        <v>8428</v>
+        <v>8422</v>
       </c>
       <c r="C7" s="2">
-        <v>60970</v>
+        <v>61224</v>
       </c>
       <c r="D7" t="s">
         <v>95</v>
@@ -1365,13 +1367,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>1382</v>
+        <v>1390</v>
       </c>
       <c r="B8" s="2">
-        <v>8705</v>
+        <v>8703</v>
       </c>
       <c r="C8" s="2">
-        <v>63185</v>
+        <v>63483</v>
       </c>
       <c r="D8" t="s">
         <v>95</v>
@@ -1399,13 +1401,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>34255</v>
+        <v>34225</v>
       </c>
       <c r="B10" s="2">
-        <v>192320</v>
+        <v>191928</v>
       </c>
       <c r="C10" s="2">
-        <v>1331670</v>
+        <v>1329140</v>
       </c>
       <c r="D10" t="s">
         <v>95</v>
@@ -1416,13 +1418,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>1331</v>
+        <v>1338</v>
       </c>
       <c r="B11" s="2">
-        <v>8449</v>
+        <v>8443</v>
       </c>
       <c r="C11" s="2">
-        <v>60986</v>
+        <v>61240</v>
       </c>
       <c r="D11" t="s">
         <v>95</v>
@@ -1433,13 +1435,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>1292</v>
+        <v>1298</v>
       </c>
       <c r="B12" s="2">
-        <v>8270</v>
+        <v>8260</v>
       </c>
       <c r="C12" s="2">
-        <v>59752</v>
+        <v>59962</v>
       </c>
       <c r="D12" t="s">
         <v>95</v>
@@ -1484,13 +1486,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>1370</v>
+        <v>1378</v>
       </c>
       <c r="B15" s="2">
-        <v>8588</v>
+        <v>8586</v>
       </c>
       <c r="C15" s="2">
-        <v>62194</v>
+        <v>62492</v>
       </c>
       <c r="D15" t="s">
         <v>95</v>
@@ -1501,13 +1503,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>1336</v>
+        <v>1343</v>
       </c>
       <c r="B16" s="2">
-        <v>8486</v>
+        <v>8480</v>
       </c>
       <c r="C16" s="2">
-        <v>61355</v>
+        <v>61609</v>
       </c>
       <c r="D16" t="s">
         <v>95</v>
@@ -1518,13 +1520,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>1380</v>
+        <v>1388</v>
       </c>
       <c r="B17" s="2">
-        <v>8685</v>
+        <v>8683</v>
       </c>
       <c r="C17" s="2">
-        <v>62939</v>
+        <v>63237</v>
       </c>
       <c r="D17" t="s">
         <v>95</v>
@@ -1535,13 +1537,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="B18" s="2">
-        <v>6032</v>
+        <v>6009</v>
       </c>
       <c r="C18" s="2">
-        <v>40615</v>
+        <v>40446</v>
       </c>
       <c r="D18" t="s">
         <v>95</v>
@@ -1552,13 +1554,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>2586</v>
+        <v>2583</v>
       </c>
       <c r="B19" s="2">
-        <v>13629</v>
+        <v>13582</v>
       </c>
       <c r="C19" s="2">
-        <v>93792</v>
+        <v>93507</v>
       </c>
       <c r="D19" t="s">
         <v>95</v>
@@ -1569,13 +1571,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>1377</v>
+        <v>1385</v>
       </c>
       <c r="B20" s="2">
-        <v>8673</v>
+        <v>8671</v>
       </c>
       <c r="C20" s="2">
-        <v>62933</v>
+        <v>63231</v>
       </c>
       <c r="D20" t="s">
         <v>95</v>
@@ -1586,13 +1588,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="B21" s="2">
-        <v>5579</v>
+        <v>5530</v>
       </c>
       <c r="C21" s="2">
-        <v>38054</v>
+        <v>37896</v>
       </c>
       <c r="D21" t="s">
         <v>95</v>
@@ -1603,13 +1605,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>33984</v>
+        <v>33979</v>
       </c>
       <c r="B22" s="2">
-        <v>177719</v>
+        <v>177528</v>
       </c>
       <c r="C22" s="2">
-        <v>1242418</v>
+        <v>1241655</v>
       </c>
       <c r="D22" t="s">
         <v>95</v>
@@ -1620,13 +1622,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B23" s="2">
-        <v>1803</v>
+        <v>1753</v>
       </c>
       <c r="C23" s="2">
-        <v>13268</v>
+        <v>13062</v>
       </c>
       <c r="D23" t="s">
         <v>95</v>
@@ -1654,13 +1656,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>1335</v>
+        <v>1342</v>
       </c>
       <c r="B25" s="2">
-        <v>8480</v>
+        <v>8474</v>
       </c>
       <c r="C25" s="2">
-        <v>61333</v>
+        <v>61587</v>
       </c>
       <c r="D25" t="s">
         <v>95</v>
@@ -1671,13 +1673,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>1333</v>
+        <v>1340</v>
       </c>
       <c r="B26" s="2">
-        <v>8436</v>
+        <v>8430</v>
       </c>
       <c r="C26" s="2">
-        <v>61060</v>
+        <v>61314</v>
       </c>
       <c r="D26" t="s">
         <v>95</v>
@@ -1705,13 +1707,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>1312</v>
+        <v>1319</v>
       </c>
       <c r="B28" s="2">
-        <v>8294</v>
+        <v>8288</v>
       </c>
       <c r="C28" s="2">
-        <v>59935</v>
+        <v>60189</v>
       </c>
       <c r="D28" t="s">
         <v>95</v>
@@ -1722,13 +1724,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>1382</v>
+        <v>1390</v>
       </c>
       <c r="B29" s="2">
-        <v>8647</v>
+        <v>8645</v>
       </c>
       <c r="C29" s="2">
-        <v>62836</v>
+        <v>63134</v>
       </c>
       <c r="D29" t="s">
         <v>95</v>
@@ -1739,13 +1741,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>1382</v>
+        <v>1390</v>
       </c>
       <c r="B30" s="2">
-        <v>8708</v>
+        <v>8706</v>
       </c>
       <c r="C30" s="2">
-        <v>63052</v>
+        <v>63350</v>
       </c>
       <c r="D30" t="s">
         <v>95</v>
@@ -1756,13 +1758,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>1318</v>
+        <v>1325</v>
       </c>
       <c r="B31" s="2">
-        <v>8316</v>
+        <v>8310</v>
       </c>
       <c r="C31" s="2">
-        <v>60158</v>
+        <v>60412</v>
       </c>
       <c r="D31" t="s">
         <v>95</v>
@@ -1773,13 +1775,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>1275</v>
+        <v>1281</v>
       </c>
       <c r="B32" s="2">
-        <v>8137</v>
+        <v>8127</v>
       </c>
       <c r="C32" s="2">
-        <v>58776</v>
+        <v>58986</v>
       </c>
       <c r="D32" t="s">
         <v>95</v>
@@ -1790,13 +1792,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>1289</v>
+        <v>1295</v>
       </c>
       <c r="B33" s="2">
-        <v>8262</v>
+        <v>8252</v>
       </c>
       <c r="C33" s="2">
-        <v>59642</v>
+        <v>59852</v>
       </c>
       <c r="D33" t="s">
         <v>95</v>
@@ -1841,13 +1843,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B36" s="2">
-        <v>6923</v>
+        <v>6913</v>
       </c>
       <c r="C36" s="2">
-        <v>47313</v>
+        <v>47260</v>
       </c>
       <c r="D36" t="s">
         <v>96</v>
@@ -1875,13 +1877,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>53340</v>
+        <v>53371</v>
       </c>
       <c r="B38" s="2">
-        <v>289377</v>
+        <v>289086</v>
       </c>
       <c r="C38" s="2">
-        <v>2002363</v>
+        <v>2001638</v>
       </c>
       <c r="D38" t="s">
         <v>96</v>
@@ -1943,13 +1945,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>8931</v>
+        <v>8941</v>
       </c>
       <c r="B42" s="2">
-        <v>54456</v>
+        <v>54504</v>
       </c>
       <c r="C42" s="2">
-        <v>370742</v>
+        <v>371488</v>
       </c>
       <c r="D42" t="s">
         <v>96</v>
@@ -2011,13 +2013,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>35206</v>
+        <v>35150</v>
       </c>
       <c r="B46" s="2">
-        <v>193931</v>
+        <v>193384</v>
       </c>
       <c r="C46" s="2">
-        <v>1346413</v>
+        <v>1342865</v>
       </c>
       <c r="D46" t="s">
         <v>97</v>
@@ -2045,13 +2047,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>2075</v>
+        <v>2072</v>
       </c>
       <c r="B48" s="2">
-        <v>10252</v>
+        <v>10230</v>
       </c>
       <c r="C48" s="2">
-        <v>69979</v>
+        <v>69768</v>
       </c>
       <c r="D48" t="s">
         <v>97</v>
@@ -2062,13 +2064,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>9886</v>
+        <v>9918</v>
       </c>
       <c r="B49" s="2">
-        <v>46798</v>
+        <v>46890</v>
       </c>
       <c r="C49" s="2">
-        <v>331998</v>
+        <v>333555</v>
       </c>
       <c r="D49" t="s">
         <v>98</v>
@@ -2130,13 +2132,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>50776</v>
+        <v>50863</v>
       </c>
       <c r="B53" s="2">
-        <v>283174</v>
+        <v>283598</v>
       </c>
       <c r="C53" s="2">
-        <v>1982569</v>
+        <v>1984961</v>
       </c>
       <c r="D53" t="s">
         <v>98</v>
@@ -2181,13 +2183,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B56" s="2">
-        <v>1705</v>
+        <v>1714</v>
       </c>
       <c r="C56" s="2">
-        <v>15615</v>
+        <v>15664</v>
       </c>
       <c r="D56" t="s">
         <v>98</v>
@@ -2215,13 +2217,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B58" s="2">
-        <v>665</v>
+        <v>656</v>
       </c>
       <c r="C58" s="2">
-        <v>5092</v>
+        <v>5036</v>
       </c>
       <c r="D58" t="s">
         <v>98</v>
@@ -2249,13 +2251,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>1647</v>
+        <v>1656</v>
       </c>
       <c r="B60" s="2">
-        <v>9421</v>
+        <v>9502</v>
       </c>
       <c r="C60" s="2">
-        <v>65662</v>
+        <v>66111</v>
       </c>
       <c r="D60" t="s">
         <v>98</v>
@@ -2266,13 +2268,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>9342</v>
+        <v>9373</v>
       </c>
       <c r="B61" s="2">
-        <v>43876</v>
+        <v>43964</v>
       </c>
       <c r="C61" s="2">
-        <v>312154</v>
+        <v>313667</v>
       </c>
       <c r="D61" t="s">
         <v>103</v>
@@ -2334,13 +2336,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>42473</v>
+        <v>46988</v>
       </c>
       <c r="B65" s="2">
-        <v>216139</v>
+        <v>259399</v>
       </c>
       <c r="C65" s="2">
-        <v>1511272</v>
+        <v>1812484</v>
       </c>
       <c r="D65" t="s">
         <v>103</v>
@@ -2368,13 +2370,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="B67" s="2">
-        <v>377</v>
+        <v>786</v>
       </c>
       <c r="C67" s="2">
-        <v>3139</v>
+        <v>5968</v>
       </c>
       <c r="D67" t="s">
         <v>103</v>
@@ -2385,13 +2387,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="B68" s="2">
-        <v>971</v>
+        <v>1527</v>
       </c>
       <c r="C68" s="2">
-        <v>7161</v>
+        <v>10679</v>
       </c>
       <c r="D68" t="s">
         <v>103</v>
@@ -2402,13 +2404,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>9688</v>
+        <v>9720</v>
       </c>
       <c r="B69" s="2">
-        <v>46430</v>
+        <v>46522</v>
       </c>
       <c r="C69" s="2">
-        <v>327338</v>
+        <v>328895</v>
       </c>
       <c r="D69" t="s">
         <v>106</v>
@@ -2453,13 +2455,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>48441</v>
+        <v>48483</v>
       </c>
       <c r="B72" s="2">
-        <v>271141</v>
+        <v>271120</v>
       </c>
       <c r="C72" s="2">
-        <v>1875698</v>
+        <v>1875638</v>
       </c>
       <c r="D72" t="s">
         <v>106</v>
@@ -2487,13 +2489,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="B74" s="2">
-        <v>6924</v>
+        <v>6914</v>
       </c>
       <c r="C74" s="2">
-        <v>47208</v>
+        <v>47155</v>
       </c>
       <c r="D74" t="s">
         <v>106</v>
@@ -2504,13 +2506,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>1620</v>
+        <v>1616</v>
       </c>
       <c r="B75" s="2">
-        <v>9764</v>
+        <v>9710</v>
       </c>
       <c r="C75" s="2">
-        <v>74876</v>
+        <v>74626</v>
       </c>
       <c r="D75" t="s">
         <v>107</v>
@@ -2521,13 +2523,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>1560</v>
+        <v>1556</v>
       </c>
       <c r="B76" s="2">
-        <v>9303</v>
+        <v>9249</v>
       </c>
       <c r="C76" s="2">
-        <v>70927</v>
+        <v>70677</v>
       </c>
       <c r="D76" t="s">
         <v>107</v>
@@ -2538,13 +2540,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>1554</v>
+        <v>1550</v>
       </c>
       <c r="B77" s="2">
-        <v>9066</v>
+        <v>9012</v>
       </c>
       <c r="C77" s="2">
-        <v>69641</v>
+        <v>69391</v>
       </c>
       <c r="D77" t="s">
         <v>107</v>
@@ -2555,13 +2557,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>1438</v>
+        <v>1434</v>
       </c>
       <c r="B78" s="2">
-        <v>8672</v>
+        <v>8618</v>
       </c>
       <c r="C78" s="2">
-        <v>65891</v>
+        <v>65641</v>
       </c>
       <c r="D78" t="s">
         <v>107</v>
@@ -2572,13 +2574,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>1667</v>
+        <v>1663</v>
       </c>
       <c r="B79" s="2">
-        <v>10154</v>
+        <v>10100</v>
       </c>
       <c r="C79" s="2">
-        <v>77719</v>
+        <v>77469</v>
       </c>
       <c r="D79" t="s">
         <v>107</v>
@@ -2606,13 +2608,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>37469</v>
+        <v>37441</v>
       </c>
       <c r="B81" s="2">
-        <v>210846</v>
+        <v>210457</v>
       </c>
       <c r="C81" s="2">
-        <v>1472288</v>
+        <v>1469793</v>
       </c>
       <c r="D81" t="s">
         <v>107</v>
@@ -2623,13 +2625,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="B82" s="2">
-        <v>8719</v>
+        <v>8665</v>
       </c>
       <c r="C82" s="2">
-        <v>65847</v>
+        <v>65597</v>
       </c>
       <c r="D82" t="s">
         <v>107</v>
@@ -2640,13 +2642,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>1799</v>
+        <v>1795</v>
       </c>
       <c r="B83" s="2">
-        <v>10318</v>
+        <v>10264</v>
       </c>
       <c r="C83" s="2">
-        <v>79599</v>
+        <v>79349</v>
       </c>
       <c r="D83" t="s">
         <v>107</v>
@@ -2657,13 +2659,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="B84" s="2">
-        <v>9505</v>
+        <v>9451</v>
       </c>
       <c r="C84" s="2">
-        <v>72840</v>
+        <v>72590</v>
       </c>
       <c r="D84" t="s">
         <v>107</v>
@@ -2674,13 +2676,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>1603</v>
+        <v>1599</v>
       </c>
       <c r="B85" s="2">
-        <v>9502</v>
+        <v>9448</v>
       </c>
       <c r="C85" s="2">
-        <v>72942</v>
+        <v>72692</v>
       </c>
       <c r="D85" t="s">
         <v>107</v>
@@ -2708,13 +2710,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>1486</v>
+        <v>1482</v>
       </c>
       <c r="B87" s="2">
-        <v>9321</v>
+        <v>9267</v>
       </c>
       <c r="C87" s="2">
-        <v>70441</v>
+        <v>70191</v>
       </c>
       <c r="D87" t="s">
         <v>107</v>
@@ -2725,13 +2727,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>1651</v>
+        <v>1647</v>
       </c>
       <c r="B88" s="2">
-        <v>9659</v>
+        <v>9605</v>
       </c>
       <c r="C88" s="2">
-        <v>74016</v>
+        <v>73766</v>
       </c>
       <c r="D88" t="s">
         <v>107</v>
@@ -2742,13 +2744,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>1702</v>
+        <v>1698</v>
       </c>
       <c r="B89" s="2">
-        <v>9836</v>
+        <v>9782</v>
       </c>
       <c r="C89" s="2">
-        <v>75723</v>
+        <v>75473</v>
       </c>
       <c r="D89" t="s">
         <v>107</v>
@@ -2759,13 +2761,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>1696</v>
+        <v>1692</v>
       </c>
       <c r="B90" s="2">
-        <v>9795</v>
+        <v>9741</v>
       </c>
       <c r="C90" s="2">
-        <v>75202</v>
+        <v>74952</v>
       </c>
       <c r="D90" t="s">
         <v>107</v>
@@ -2776,13 +2778,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>1555</v>
+        <v>1551</v>
       </c>
       <c r="B91" s="2">
-        <v>9077</v>
+        <v>9023</v>
       </c>
       <c r="C91" s="2">
-        <v>69737</v>
+        <v>69487</v>
       </c>
       <c r="D91" t="s">
         <v>107</v>
@@ -2793,13 +2795,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>1645</v>
+        <v>1641</v>
       </c>
       <c r="B92" s="2">
-        <v>9625</v>
+        <v>9571</v>
       </c>
       <c r="C92" s="2">
-        <v>73968</v>
+        <v>73718</v>
       </c>
       <c r="D92" t="s">
         <v>107</v>
@@ -2810,13 +2812,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>1713</v>
+        <v>1707</v>
       </c>
       <c r="B93" s="2">
-        <v>6082</v>
+        <v>6030</v>
       </c>
       <c r="C93" s="2">
-        <v>42337</v>
+        <v>42096</v>
       </c>
       <c r="D93" t="s">
         <v>107</v>
@@ -2827,13 +2829,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>29490</v>
+        <v>29437</v>
       </c>
       <c r="B94" s="2">
-        <v>141291</v>
+        <v>140856</v>
       </c>
       <c r="C94" s="2">
-        <v>1012065</v>
+        <v>1009246</v>
       </c>
       <c r="D94" t="s">
         <v>107</v>
@@ -2844,13 +2846,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>38769</v>
+        <v>38756</v>
       </c>
       <c r="B95" s="2">
-        <v>204855</v>
+        <v>204633</v>
       </c>
       <c r="C95" s="2">
-        <v>1447580</v>
+        <v>1446469</v>
       </c>
       <c r="D95" t="s">
         <v>107</v>
@@ -2861,13 +2863,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>4887</v>
+        <v>4900</v>
       </c>
       <c r="B96" s="2">
-        <v>27882</v>
+        <v>27913</v>
       </c>
       <c r="C96" s="2">
-        <v>198293</v>
+        <v>198800</v>
       </c>
       <c r="D96" t="s">
         <v>112</v>
@@ -2878,13 +2880,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B97" s="2">
-        <v>1938</v>
+        <v>1884</v>
       </c>
       <c r="C97" s="2">
-        <v>14271</v>
+        <v>14021</v>
       </c>
       <c r="D97" t="s">
         <v>107</v>
@@ -2912,13 +2914,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>1512</v>
+        <v>1508</v>
       </c>
       <c r="B99" s="2">
-        <v>9092</v>
+        <v>9038</v>
       </c>
       <c r="C99" s="2">
-        <v>69293</v>
+        <v>69043</v>
       </c>
       <c r="D99" t="s">
         <v>107</v>
@@ -2929,13 +2931,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>60197</v>
+        <v>60163</v>
       </c>
       <c r="B100" s="2">
-        <v>315054</v>
+        <v>314583</v>
       </c>
       <c r="C100" s="2">
-        <v>2217886</v>
+        <v>2215017</v>
       </c>
       <c r="D100" t="s">
         <v>112</v>
@@ -2946,13 +2948,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>1475</v>
+        <v>1471</v>
       </c>
       <c r="B101" s="2">
-        <v>8783</v>
+        <v>8729</v>
       </c>
       <c r="C101" s="2">
-        <v>66992</v>
+        <v>66742</v>
       </c>
       <c r="D101" t="s">
         <v>107</v>
@@ -2963,13 +2965,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>1592</v>
+        <v>1588</v>
       </c>
       <c r="B102" s="2">
-        <v>9357</v>
+        <v>9303</v>
       </c>
       <c r="C102" s="2">
-        <v>71833</v>
+        <v>71583</v>
       </c>
       <c r="D102" t="s">
         <v>107</v>
@@ -2980,13 +2982,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>1640</v>
+        <v>1636</v>
       </c>
       <c r="B103" s="2">
-        <v>9591</v>
+        <v>9537</v>
       </c>
       <c r="C103" s="2">
-        <v>73458</v>
+        <v>73208</v>
       </c>
       <c r="D103" t="s">
         <v>107</v>
@@ -2997,13 +2999,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>1729</v>
+        <v>1725</v>
       </c>
       <c r="B104" s="2">
-        <v>10041</v>
+        <v>9987</v>
       </c>
       <c r="C104" s="2">
-        <v>77229</v>
+        <v>76979</v>
       </c>
       <c r="D104" t="s">
         <v>107</v>
@@ -3014,13 +3016,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>3379</v>
+        <v>3392</v>
       </c>
       <c r="B105" s="2">
-        <v>17604</v>
+        <v>17564</v>
       </c>
       <c r="C105" s="2">
-        <v>125170</v>
+        <v>124871</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -3031,13 +3033,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="B106" s="2">
-        <v>9421</v>
+        <v>9367</v>
       </c>
       <c r="C106" s="2">
-        <v>72216</v>
+        <v>71966</v>
       </c>
       <c r="D106" t="s">
         <v>107</v>
@@ -3048,13 +3050,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>1563</v>
+        <v>1559</v>
       </c>
       <c r="B107" s="2">
-        <v>9488</v>
+        <v>9434</v>
       </c>
       <c r="C107" s="2">
-        <v>72248</v>
+        <v>71998</v>
       </c>
       <c r="D107" t="s">
         <v>107</v>
@@ -3065,13 +3067,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="B108" s="2">
-        <v>8974</v>
+        <v>8920</v>
       </c>
       <c r="C108" s="2">
-        <v>68272</v>
+        <v>68022</v>
       </c>
       <c r="D108" t="s">
         <v>107</v>
@@ -3099,13 +3101,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>20114</v>
+        <v>20102</v>
       </c>
       <c r="B110" s="2">
-        <v>113474</v>
+        <v>113356</v>
       </c>
       <c r="C110" s="2">
-        <v>795861</v>
+        <v>795201</v>
       </c>
       <c r="D110" t="s">
         <v>108</v>
@@ -3116,13 +3118,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>15374</v>
+        <v>15370</v>
       </c>
       <c r="B111" s="2">
-        <v>85480</v>
+        <v>85452</v>
       </c>
       <c r="C111" s="2">
-        <v>597137</v>
+        <v>596941</v>
       </c>
       <c r="D111" t="s">
         <v>108</v>
@@ -3167,13 +3169,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>14656</v>
+        <v>14703</v>
       </c>
       <c r="B114" s="2">
-        <v>90362</v>
+        <v>90563</v>
       </c>
       <c r="C114" s="2">
-        <v>624169</v>
+        <v>626359</v>
       </c>
       <c r="D114" t="s">
         <v>108</v>
@@ -3184,13 +3186,13 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>24512</v>
+        <v>24518</v>
       </c>
       <c r="B115" s="2">
-        <v>142129</v>
+        <v>142141</v>
       </c>
       <c r="C115" s="2">
-        <v>982848</v>
+        <v>983032</v>
       </c>
       <c r="D115" t="s">
         <v>108</v>
@@ -3201,13 +3203,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>18709</v>
+        <v>18766</v>
       </c>
       <c r="B116" s="2">
-        <v>70132</v>
+        <v>70564</v>
       </c>
       <c r="C116" s="2">
-        <v>506712</v>
+        <v>509622</v>
       </c>
       <c r="D116" t="s">
         <v>108</v>
@@ -3235,13 +3237,13 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>6462</v>
+        <v>6373</v>
       </c>
       <c r="B118" s="2">
-        <v>27663</v>
+        <v>26970</v>
       </c>
       <c r="C118" s="2">
-        <v>214850</v>
+        <v>210083</v>
       </c>
       <c r="D118" t="s">
         <v>108</v>
@@ -3563,7 +3565,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>157013</v>
+        <v>156561</v>
       </c>
       <c r="B4" t="s">
         <v>94</v>
@@ -3585,7 +3587,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>13545</v>
+        <v>13496</v>
       </c>
       <c r="B6" t="s">
         <v>94</v>
@@ -3596,7 +3598,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>3221</v>
+        <v>3208</v>
       </c>
       <c r="B7" t="s">
         <v>95</v>
@@ -3607,7 +3609,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>3412</v>
+        <v>3402</v>
       </c>
       <c r="B8" t="s">
         <v>95</v>
@@ -3629,7 +3631,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>147303</v>
+        <v>146936</v>
       </c>
       <c r="B10" t="s">
         <v>95</v>
@@ -3640,7 +3642,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>3220</v>
+        <v>3207</v>
       </c>
       <c r="B11" t="s">
         <v>95</v>
@@ -3651,7 +3653,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>3075</v>
+        <v>3059</v>
       </c>
       <c r="B12" t="s">
         <v>95</v>
@@ -3684,7 +3686,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>3382</v>
+        <v>3372</v>
       </c>
       <c r="B15" t="s">
         <v>95</v>
@@ -3695,7 +3697,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>3229</v>
+        <v>3216</v>
       </c>
       <c r="B16" t="s">
         <v>95</v>
@@ -3706,7 +3708,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>3378</v>
+        <v>3368</v>
       </c>
       <c r="B17" t="s">
         <v>95</v>
@@ -3717,7 +3719,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>3318</v>
+        <v>3297</v>
       </c>
       <c r="B18" t="s">
         <v>95</v>
@@ -3728,7 +3730,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>9678</v>
+        <v>9634</v>
       </c>
       <c r="B19" t="s">
         <v>95</v>
@@ -3739,7 +3741,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>3410</v>
+        <v>3400</v>
       </c>
       <c r="B20" t="s">
         <v>95</v>
@@ -3750,7 +3752,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>2064</v>
+        <v>2018</v>
       </c>
       <c r="B21" t="s">
         <v>95</v>
@@ -3761,7 +3763,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>125471</v>
+        <v>125281</v>
       </c>
       <c r="B22" t="s">
         <v>95</v>
@@ -3772,7 +3774,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>832</v>
+        <v>785</v>
       </c>
       <c r="B23" t="s">
         <v>95</v>
@@ -3794,7 +3796,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>3239</v>
+        <v>3226</v>
       </c>
       <c r="B25" t="s">
         <v>95</v>
@@ -3805,7 +3807,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>3239</v>
+        <v>3226</v>
       </c>
       <c r="B26" t="s">
         <v>95</v>
@@ -3827,7 +3829,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>3197</v>
+        <v>3184</v>
       </c>
       <c r="B28" t="s">
         <v>95</v>
@@ -3838,7 +3840,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>3390</v>
+        <v>3380</v>
       </c>
       <c r="B29" t="s">
         <v>95</v>
@@ -3849,7 +3851,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>3410</v>
+        <v>3400</v>
       </c>
       <c r="B30" t="s">
         <v>95</v>
@@ -3860,7 +3862,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>3216</v>
+        <v>3203</v>
       </c>
       <c r="B31" t="s">
         <v>95</v>
@@ -3871,7 +3873,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>3050</v>
+        <v>3034</v>
       </c>
       <c r="B32" t="s">
         <v>95</v>
@@ -3882,7 +3884,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>3077</v>
+        <v>3061</v>
       </c>
       <c r="B33" t="s">
         <v>95</v>
@@ -3915,7 +3917,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>5057</v>
+        <v>5048</v>
       </c>
       <c r="B36" t="s">
         <v>96</v>
@@ -3937,7 +3939,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>196285</v>
+        <v>195949</v>
       </c>
       <c r="B38" t="s">
         <v>96</v>
@@ -3981,7 +3983,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>42232</v>
+        <v>42263</v>
       </c>
       <c r="B42" t="s">
         <v>96</v>
@@ -4025,7 +4027,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>142629</v>
+        <v>142136</v>
       </c>
       <c r="B46" t="s">
         <v>97</v>
@@ -4047,7 +4049,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>7416</v>
+        <v>7397</v>
       </c>
       <c r="B48" t="s">
         <v>97</v>
@@ -4058,7 +4060,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>16301</v>
+        <v>16359</v>
       </c>
       <c r="B49" t="s">
         <v>98</v>
@@ -4102,7 +4104,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>215405</v>
+        <v>215731</v>
       </c>
       <c r="B53" t="s">
         <v>98</v>
@@ -4135,7 +4137,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>787</v>
+        <v>795</v>
       </c>
       <c r="B56" t="s">
         <v>98</v>
@@ -4179,7 +4181,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>5984</v>
+        <v>6056</v>
       </c>
       <c r="B60" t="s">
         <v>98</v>
@@ -4190,7 +4192,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>15419</v>
+        <v>15474</v>
       </c>
       <c r="B61" t="s">
         <v>103</v>
@@ -4234,7 +4236,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>160521</v>
+        <v>198110</v>
       </c>
       <c r="B65" t="s">
         <v>103</v>
@@ -4256,7 +4258,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>189</v>
+        <v>532</v>
       </c>
       <c r="B67" t="s">
         <v>103</v>
@@ -4267,7 +4269,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>328</v>
+        <v>826</v>
       </c>
       <c r="B68" t="s">
         <v>103</v>
@@ -4278,7 +4280,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>16105</v>
+        <v>16163</v>
       </c>
       <c r="B69" t="s">
         <v>106</v>
@@ -4311,7 +4313,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>205992</v>
+        <v>205914</v>
       </c>
       <c r="B72" t="s">
         <v>106</v>
@@ -4333,7 +4335,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>5159</v>
+        <v>5150</v>
       </c>
       <c r="B74" t="s">
         <v>106</v>
@@ -4344,7 +4346,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>4489</v>
+        <v>4439</v>
       </c>
       <c r="B75" t="s">
         <v>107</v>
@@ -4355,7 +4357,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>3923</v>
+        <v>3873</v>
       </c>
       <c r="B76" t="s">
         <v>107</v>
@@ -4366,7 +4368,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>3890</v>
+        <v>3840</v>
       </c>
       <c r="B77" t="s">
         <v>107</v>
@@ -4377,7 +4379,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>3601</v>
+        <v>3551</v>
       </c>
       <c r="B78" t="s">
         <v>107</v>
@@ -4388,7 +4390,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>4877</v>
+        <v>4827</v>
       </c>
       <c r="B79" t="s">
         <v>107</v>
@@ -4410,7 +4412,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>163672</v>
+        <v>163303</v>
       </c>
       <c r="B81" t="s">
         <v>107</v>
@@ -4421,7 +4423,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>3518</v>
+        <v>3468</v>
       </c>
       <c r="B82" t="s">
         <v>107</v>
@@ -4432,7 +4434,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>4829</v>
+        <v>4779</v>
       </c>
       <c r="B83" t="s">
         <v>107</v>
@@ -4443,7 +4445,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>4202</v>
+        <v>4152</v>
       </c>
       <c r="B84" t="s">
         <v>107</v>
@@ -4454,7 +4456,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>4237</v>
+        <v>4187</v>
       </c>
       <c r="B85" t="s">
         <v>107</v>
@@ -4476,7 +4478,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>4139</v>
+        <v>4089</v>
       </c>
       <c r="B87" t="s">
         <v>107</v>
@@ -4487,7 +4489,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>4237</v>
+        <v>4187</v>
       </c>
       <c r="B88" t="s">
         <v>107</v>
@@ -4498,7 +4500,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>4582</v>
+        <v>4532</v>
       </c>
       <c r="B89" t="s">
         <v>107</v>
@@ -4509,7 +4511,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>4339</v>
+        <v>4289</v>
       </c>
       <c r="B90" t="s">
         <v>107</v>
@@ -4520,7 +4522,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>3895</v>
+        <v>3845</v>
       </c>
       <c r="B91" t="s">
         <v>107</v>
@@ -4531,7 +4533,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>4169</v>
+        <v>4119</v>
       </c>
       <c r="B92" t="s">
         <v>107</v>
@@ -4542,7 +4544,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>2415</v>
+        <v>2369</v>
       </c>
       <c r="B93" t="s">
         <v>107</v>
@@ -4553,7 +4555,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>95390</v>
+        <v>95003</v>
       </c>
       <c r="B94" t="s">
         <v>107</v>
@@ -4564,7 +4566,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>148763</v>
+        <v>148550</v>
       </c>
       <c r="B95" t="s">
         <v>107</v>
@@ -4575,7 +4577,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>21706</v>
+        <v>21719</v>
       </c>
       <c r="B96" t="s">
         <v>112</v>
@@ -4586,7 +4588,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>962</v>
+        <v>912</v>
       </c>
       <c r="B97" t="s">
         <v>107</v>
@@ -4608,7 +4610,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>3785</v>
+        <v>3735</v>
       </c>
       <c r="B99" t="s">
         <v>107</v>
@@ -4619,7 +4621,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>210428</v>
+        <v>209989</v>
       </c>
       <c r="B100" t="s">
         <v>112</v>
@@ -4630,7 +4632,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>3701</v>
+        <v>3651</v>
       </c>
       <c r="B101" t="s">
         <v>107</v>
@@ -4641,7 +4643,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>4003</v>
+        <v>3953</v>
       </c>
       <c r="B102" t="s">
         <v>107</v>
@@ -4652,7 +4654,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>4171</v>
+        <v>4121</v>
       </c>
       <c r="B103" t="s">
         <v>107</v>
@@ -4663,7 +4665,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>4633</v>
+        <v>4583</v>
       </c>
       <c r="B104" t="s">
         <v>107</v>
@@ -4674,7 +4676,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>13269</v>
+        <v>13214</v>
       </c>
       <c r="B105" t="s">
         <v>107</v>
@@ -4685,7 +4687,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>4143</v>
+        <v>4093</v>
       </c>
       <c r="B106" t="s">
         <v>107</v>
@@ -4696,7 +4698,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>4183</v>
+        <v>4133</v>
       </c>
       <c r="B107" t="s">
         <v>107</v>
@@ -4707,7 +4709,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>3726</v>
+        <v>3676</v>
       </c>
       <c r="B108" t="s">
         <v>107</v>
@@ -4729,7 +4731,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>85055</v>
+        <v>84949</v>
       </c>
       <c r="B110" t="s">
         <v>108</v>
@@ -4740,7 +4742,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>60301</v>
+        <v>60277</v>
       </c>
       <c r="B111" t="s">
         <v>108</v>
@@ -4773,7 +4775,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>60101</v>
+        <v>60255</v>
       </c>
       <c r="B114" t="s">
         <v>108</v>
@@ -4784,7 +4786,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>109544</v>
+        <v>109548</v>
       </c>
       <c r="B115" t="s">
         <v>108</v>
@@ -4795,7 +4797,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>31203</v>
+        <v>31558</v>
       </c>
       <c r="B116" t="s">
         <v>108</v>
@@ -4817,7 +4819,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>19922</v>
+        <v>19318</v>
       </c>
       <c r="B118" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
Update code analysis scripts to include The Sentinel
</commit_message>
<xml_diff>
--- a/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
+++ b/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mark/Documents/Files/Websites/Repositories/bbcelite-scripts/code-analysis/word-count-code-comments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C484A8C4-7810-7F47-B1E7-1B2897E32B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6755AB8-43A0-C447-B0F7-0647BFADA7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="2800" windowWidth="21600" windowHeight="17440" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
+    <workbookView xWindow="17280" yWindow="2800" windowWidth="21580" windowHeight="17800" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="119">
   <si>
     <t>Lines</t>
   </si>
@@ -381,6 +381,18 @@
   </si>
   <si>
     <t>elite-sprites.asm</t>
+  </si>
+  <si>
+    <t>the-sentinel-source-code-bbc-micro</t>
+  </si>
+  <si>
+    <t>the-sentinel-build-options.asm</t>
+  </si>
+  <si>
+    <t>the-sentinel-source.asm</t>
+  </si>
+  <si>
+    <t>the-sentinel-disc.asm</t>
   </si>
 </sst>
 </file>
@@ -771,7 +783,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4742C6F-ED5A-B74D-BFAE-09A904247301}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -805,15 +817,15 @@
       </c>
       <c r="B2" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A2,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$I$4</f>
-        <v>151416</v>
+        <v>151589</v>
       </c>
       <c r="C2" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A2)</f>
-        <v>518175</v>
+        <v>519881</v>
       </c>
       <c r="D2" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A2)</f>
-        <v>798332</v>
+        <v>800265</v>
       </c>
       <c r="H2" t="s">
         <v>81</v>
@@ -829,15 +841,15 @@
       </c>
       <c r="B3" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A3,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>113986</v>
+        <v>114088</v>
       </c>
       <c r="C3" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A3)</f>
-        <v>399844</v>
+        <v>400766</v>
       </c>
       <c r="D3" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A3)</f>
-        <v>622052</v>
+        <v>623092</v>
       </c>
       <c r="H3" t="s">
         <v>83</v>
@@ -853,15 +865,15 @@
       </c>
       <c r="B4" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A4,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$I$8</f>
-        <v>100881</v>
+        <v>100991</v>
       </c>
       <c r="C4" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A4)</f>
-        <v>348255</v>
+        <v>349369</v>
       </c>
       <c r="D4" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A4)</f>
-        <v>543268</v>
+        <v>544543</v>
       </c>
       <c r="H4" t="s">
         <v>86</v>
@@ -877,15 +889,15 @@
       </c>
       <c r="B5" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A5,linecount.txt!E:E,"&lt;&gt;revs-build-options.asm",linecount.txt!E:E,"&lt;&gt;revs-disc.asm")</f>
-        <v>67526</v>
+        <v>67559</v>
       </c>
       <c r="C5" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A5)</f>
-        <v>269887</v>
+        <v>270219</v>
       </c>
       <c r="D5" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A5)</f>
-        <v>368850</v>
+        <v>369255</v>
       </c>
       <c r="I5" s="4"/>
     </row>
@@ -895,15 +907,15 @@
       </c>
       <c r="B6" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A6,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>66168</v>
+        <v>66278</v>
       </c>
       <c r="C6" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A6)</f>
-        <v>247241</v>
+        <v>248188</v>
       </c>
       <c r="D6" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A6)</f>
-        <v>354803</v>
+        <v>355882</v>
       </c>
       <c r="H6" t="s">
         <v>82</v>
@@ -919,15 +931,15 @@
       </c>
       <c r="B7" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A7,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>65071</v>
+        <v>65169</v>
       </c>
       <c r="C7" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A7)</f>
-        <v>231876</v>
+        <v>232712</v>
       </c>
       <c r="D7" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A7)</f>
-        <v>342675</v>
+        <v>343621</v>
       </c>
       <c r="H7" t="s">
         <v>85</v>
@@ -943,15 +955,15 @@
       </c>
       <c r="B8" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A8,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>64467</v>
+        <v>64571</v>
       </c>
       <c r="C8" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A8)</f>
-        <v>245454</v>
+        <v>246415</v>
       </c>
       <c r="D8" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A8)</f>
-        <v>354855</v>
+        <v>355943</v>
       </c>
       <c r="H8" t="s">
         <v>86</v>
@@ -967,15 +979,15 @@
       </c>
       <c r="B9" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A9,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>60267</v>
+        <v>60366</v>
       </c>
       <c r="C9" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A9)</f>
-        <v>228445</v>
+        <v>229336</v>
       </c>
       <c r="D9" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A9)</f>
-        <v>324813</v>
+        <v>325822</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -985,15 +997,15 @@
       </c>
       <c r="B10" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A10,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>59511</v>
+        <v>59626</v>
       </c>
       <c r="C10" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A10)</f>
-        <v>227662</v>
+        <v>228717</v>
       </c>
       <c r="D10" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A10)</f>
-        <v>325235</v>
+        <v>325884</v>
       </c>
       <c r="H10" t="s">
         <v>84</v>
@@ -1006,15 +1018,15 @@
       </c>
       <c r="B11" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A11,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>41761</v>
+        <v>41863</v>
       </c>
       <c r="C11" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A11)</f>
-        <v>171162</v>
+        <v>172072</v>
       </c>
       <c r="D11" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A11)</f>
-        <v>231926</v>
+        <v>232952</v>
       </c>
       <c r="H11" t="s">
         <v>2</v>
@@ -1026,19 +1038,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B12" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A12,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
-        <v>37371</v>
+        <v>41020</v>
       </c>
       <c r="C12" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A12)</f>
-        <v>150107</v>
+        <v>178109</v>
       </c>
       <c r="D12" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A12)</f>
-        <v>204665</v>
+        <v>239380</v>
       </c>
       <c r="H12" t="s">
         <v>8</v>
@@ -1050,179 +1062,196 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B13" s="4">
-        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A13,linecount.txt!E:E,"&lt;&gt;aviator-build-options.asm",linecount.txt!E:E,"&lt;&gt;aviator-disc.asm",linecount.txt!E:E,"&lt;&gt;aviator-readme.asm")</f>
-        <v>31403</v>
+        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A13,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
+        <v>37476</v>
       </c>
       <c r="C13" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A13)</f>
-        <v>133457</v>
+        <v>151004</v>
       </c>
       <c r="D13" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A13)</f>
-        <v>178209</v>
+        <v>205681</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14" s="4">
-        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A14,linecount.txt!E:E,"&lt;&gt;revs-build-options.asm",linecount.txt!E:E,"&lt;&gt;revs-disc.asm")</f>
-        <v>15252</v>
+        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A14,linecount.txt!E:E,"&lt;&gt;aviator-build-options.asm",linecount.txt!E:E,"&lt;&gt;aviator-disc.asm",linecount.txt!E:E,"&lt;&gt;aviator-readme.asm")</f>
+        <v>31407</v>
       </c>
       <c r="C14" s="4">
         <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A14)</f>
-        <v>52961</v>
+        <v>133534</v>
       </c>
       <c r="D14" s="4">
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A14)</f>
-        <v>83659</v>
+        <v>178304</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="5">
-        <f>SUM(B2:B14)</f>
-        <v>875080</v>
-      </c>
-      <c r="C15" s="5">
-        <f>SUM(C2:C14)</f>
-        <v>3224526</v>
-      </c>
-      <c r="D15" s="5">
-        <f>SUM(D2:D14)</f>
-        <v>4733342</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="4">
+        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A15,linecount.txt!E:E,"&lt;&gt;revs-build-options.asm",linecount.txt!E:E,"&lt;&gt;revs-disc.asm")</f>
+        <v>15270</v>
+      </c>
+      <c r="C15" s="4">
+        <f>SUMIFS(wordcount.txt!A:A,wordcount.txt!B:B,Totals!$A15)</f>
+        <v>53052</v>
+      </c>
+      <c r="D15" s="4">
+        <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A15)</f>
+        <v>83770</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="5">
+        <f>SUM(B2:B15)</f>
+        <v>917273</v>
+      </c>
+      <c r="C16" s="5">
+        <f>SUM(C2:C15)</f>
+        <v>3413374</v>
+      </c>
+      <c r="D16" s="5">
+        <f>SUM(D2:D15)</f>
+        <v>4984394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="4">
-        <v>455125</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="4">
-        <v>587287</v>
+        <v>455125</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="4">
-        <v>211591</v>
+        <v>587287</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="4">
+        <v>211591</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C24" s="4">
         <v>783137</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="5">
-        <f>SUM(C20:C23)</f>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="5">
+        <f>SUM(C21:C24)</f>
         <v>2037140</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="4"/>
-    </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="4">
-        <v>77325</v>
-      </c>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="4">
-        <v>84799</v>
+        <v>77325</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="4">
-        <v>106821</v>
+        <v>84799</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="4">
-        <v>190858</v>
+        <v>106821</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="4">
-        <v>257154</v>
+        <v>190858</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" s="4">
-        <v>169441</v>
+        <v>257154</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="4">
+        <v>169441</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C33" s="4">
         <v>198227</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="5">
-        <f>SUM(C26:C32)</f>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="5">
+        <f>SUM(C27:C33)</f>
         <v>1084625</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C36" s="6">
         <v>835997</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D13">
-    <sortCondition descending="1" ref="B2:B13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D14">
+    <sortCondition descending="1" ref="B2:B14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1231,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A41BAD4-CFE1-7E43-9F45-0738248790D4}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E135"/>
+      <selection sqref="A1:E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,10 +1295,10 @@
         <v>251</v>
       </c>
       <c r="B2" s="2">
-        <v>1041</v>
+        <v>1048</v>
       </c>
       <c r="C2" s="2">
-        <v>8058</v>
+        <v>8107</v>
       </c>
       <c r="D2" t="s">
         <v>94</v>
@@ -1297,13 +1326,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>38142</v>
+        <v>38244</v>
       </c>
       <c r="B4" s="2">
-        <v>212320</v>
+        <v>213311</v>
       </c>
       <c r="C4" s="2">
-        <v>1473607</v>
+        <v>1480763</v>
       </c>
       <c r="D4" t="s">
         <v>94</v>
@@ -1334,10 +1363,10 @@
         <v>3368</v>
       </c>
       <c r="B6" s="2">
-        <v>18044</v>
+        <v>18072</v>
       </c>
       <c r="C6" s="2">
-        <v>124755</v>
+        <v>124951</v>
       </c>
       <c r="D6" t="s">
         <v>94</v>
@@ -1351,10 +1380,10 @@
         <v>1335</v>
       </c>
       <c r="B7" s="2">
-        <v>8422</v>
+        <v>8429</v>
       </c>
       <c r="C7" s="2">
-        <v>61224</v>
+        <v>61273</v>
       </c>
       <c r="D7" t="s">
         <v>95</v>
@@ -1368,10 +1397,10 @@
         <v>1390</v>
       </c>
       <c r="B8" s="2">
-        <v>8703</v>
+        <v>8710</v>
       </c>
       <c r="C8" s="2">
-        <v>63483</v>
+        <v>63532</v>
       </c>
       <c r="D8" t="s">
         <v>95</v>
@@ -1399,13 +1428,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>34232</v>
+        <v>34328</v>
       </c>
       <c r="B10" s="2">
-        <v>192088</v>
+        <v>192980</v>
       </c>
       <c r="C10" s="2">
-        <v>1330223</v>
+        <v>1336773</v>
       </c>
       <c r="D10" t="s">
         <v>95</v>
@@ -1419,10 +1448,10 @@
         <v>1338</v>
       </c>
       <c r="B11" s="2">
-        <v>8443</v>
+        <v>8450</v>
       </c>
       <c r="C11" s="2">
-        <v>61240</v>
+        <v>61289</v>
       </c>
       <c r="D11" t="s">
         <v>95</v>
@@ -1436,10 +1465,10 @@
         <v>1298</v>
       </c>
       <c r="B12" s="2">
-        <v>8260</v>
+        <v>8267</v>
       </c>
       <c r="C12" s="2">
-        <v>59962</v>
+        <v>60011</v>
       </c>
       <c r="D12" t="s">
         <v>95</v>
@@ -1453,10 +1482,10 @@
         <v>492</v>
       </c>
       <c r="B13" s="2">
-        <v>2342</v>
+        <v>2356</v>
       </c>
       <c r="C13" s="2">
-        <v>17676</v>
+        <v>17774</v>
       </c>
       <c r="D13" t="s">
         <v>95</v>
@@ -1487,10 +1516,10 @@
         <v>1378</v>
       </c>
       <c r="B15" s="2">
-        <v>8586</v>
+        <v>8593</v>
       </c>
       <c r="C15" s="2">
-        <v>62492</v>
+        <v>62541</v>
       </c>
       <c r="D15" t="s">
         <v>95</v>
@@ -1504,10 +1533,10 @@
         <v>1343</v>
       </c>
       <c r="B16" s="2">
-        <v>8480</v>
+        <v>8487</v>
       </c>
       <c r="C16" s="2">
-        <v>61609</v>
+        <v>61658</v>
       </c>
       <c r="D16" t="s">
         <v>95</v>
@@ -1521,10 +1550,10 @@
         <v>1388</v>
       </c>
       <c r="B17" s="2">
-        <v>8683</v>
+        <v>8690</v>
       </c>
       <c r="C17" s="2">
-        <v>63237</v>
+        <v>63286</v>
       </c>
       <c r="D17" t="s">
         <v>95</v>
@@ -1538,10 +1567,10 @@
         <v>1520</v>
       </c>
       <c r="B18" s="2">
-        <v>6009</v>
+        <v>6044</v>
       </c>
       <c r="C18" s="2">
-        <v>40446</v>
+        <v>40691</v>
       </c>
       <c r="D18" t="s">
         <v>95</v>
@@ -1552,13 +1581,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>2585</v>
+        <v>2591</v>
       </c>
       <c r="B19" s="2">
-        <v>13607</v>
+        <v>13674</v>
       </c>
       <c r="C19" s="2">
-        <v>93636</v>
+        <v>94075</v>
       </c>
       <c r="D19" t="s">
         <v>95</v>
@@ -1572,10 +1601,10 @@
         <v>1385</v>
       </c>
       <c r="B20" s="2">
-        <v>8671</v>
+        <v>8678</v>
       </c>
       <c r="C20" s="2">
-        <v>63231</v>
+        <v>63280</v>
       </c>
       <c r="D20" t="s">
         <v>95</v>
@@ -1589,10 +1618,10 @@
         <v>1577</v>
       </c>
       <c r="B21" s="2">
-        <v>5530</v>
+        <v>5537</v>
       </c>
       <c r="C21" s="2">
-        <v>37896</v>
+        <v>37945</v>
       </c>
       <c r="D21" t="s">
         <v>95</v>
@@ -1603,13 +1632,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>33988</v>
+        <v>33996</v>
       </c>
       <c r="B22" s="2">
-        <v>177697</v>
+        <v>177824</v>
       </c>
       <c r="C22" s="2">
-        <v>1242870</v>
+        <v>1243784</v>
       </c>
       <c r="D22" t="s">
         <v>95</v>
@@ -1623,10 +1652,10 @@
         <v>381</v>
       </c>
       <c r="B23" s="2">
-        <v>1753</v>
+        <v>1760</v>
       </c>
       <c r="C23" s="2">
-        <v>13062</v>
+        <v>13111</v>
       </c>
       <c r="D23" t="s">
         <v>95</v>
@@ -1657,10 +1686,10 @@
         <v>1342</v>
       </c>
       <c r="B25" s="2">
-        <v>8474</v>
+        <v>8481</v>
       </c>
       <c r="C25" s="2">
-        <v>61587</v>
+        <v>61636</v>
       </c>
       <c r="D25" t="s">
         <v>95</v>
@@ -1674,10 +1703,10 @@
         <v>1340</v>
       </c>
       <c r="B26" s="2">
-        <v>8430</v>
+        <v>8437</v>
       </c>
       <c r="C26" s="2">
-        <v>61314</v>
+        <v>61363</v>
       </c>
       <c r="D26" t="s">
         <v>95</v>
@@ -1691,10 +1720,10 @@
         <v>1542</v>
       </c>
       <c r="B27" s="2">
-        <v>8156</v>
+        <v>8170</v>
       </c>
       <c r="C27" s="2">
-        <v>60139</v>
+        <v>60237</v>
       </c>
       <c r="D27" t="s">
         <v>95</v>
@@ -1708,10 +1737,10 @@
         <v>1319</v>
       </c>
       <c r="B28" s="2">
-        <v>8288</v>
+        <v>8295</v>
       </c>
       <c r="C28" s="2">
-        <v>60189</v>
+        <v>60238</v>
       </c>
       <c r="D28" t="s">
         <v>95</v>
@@ -1725,10 +1754,10 @@
         <v>1390</v>
       </c>
       <c r="B29" s="2">
-        <v>8645</v>
+        <v>8652</v>
       </c>
       <c r="C29" s="2">
-        <v>63134</v>
+        <v>63183</v>
       </c>
       <c r="D29" t="s">
         <v>95</v>
@@ -1742,10 +1771,10 @@
         <v>1390</v>
       </c>
       <c r="B30" s="2">
-        <v>8706</v>
+        <v>8713</v>
       </c>
       <c r="C30" s="2">
-        <v>63350</v>
+        <v>63399</v>
       </c>
       <c r="D30" t="s">
         <v>95</v>
@@ -1759,10 +1788,10 @@
         <v>1325</v>
       </c>
       <c r="B31" s="2">
-        <v>8310</v>
+        <v>8317</v>
       </c>
       <c r="C31" s="2">
-        <v>60412</v>
+        <v>60461</v>
       </c>
       <c r="D31" t="s">
         <v>95</v>
@@ -1776,10 +1805,10 @@
         <v>1281</v>
       </c>
       <c r="B32" s="2">
-        <v>8127</v>
+        <v>8134</v>
       </c>
       <c r="C32" s="2">
-        <v>58986</v>
+        <v>59035</v>
       </c>
       <c r="D32" t="s">
         <v>95</v>
@@ -1793,10 +1822,10 @@
         <v>1295</v>
       </c>
       <c r="B33" s="2">
-        <v>8252</v>
+        <v>8259</v>
       </c>
       <c r="C33" s="2">
-        <v>59852</v>
+        <v>59901</v>
       </c>
       <c r="D33" t="s">
         <v>95</v>
@@ -1827,10 +1856,10 @@
         <v>314</v>
       </c>
       <c r="B35" s="2">
-        <v>1522</v>
+        <v>1529</v>
       </c>
       <c r="C35" s="2">
-        <v>9451</v>
+        <v>9500</v>
       </c>
       <c r="D35" t="s">
         <v>96</v>
@@ -1844,10 +1873,10 @@
         <v>1336</v>
       </c>
       <c r="B36" s="2">
-        <v>6916</v>
+        <v>6930</v>
       </c>
       <c r="C36" s="2">
-        <v>47283</v>
+        <v>47381</v>
       </c>
       <c r="D36" t="s">
         <v>96</v>
@@ -1875,13 +1904,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>53375</v>
+        <v>53479</v>
       </c>
       <c r="B38" s="2">
-        <v>289221</v>
+        <v>290239</v>
       </c>
       <c r="C38" s="2">
-        <v>2002565</v>
+        <v>2010000</v>
       </c>
       <c r="D38" t="s">
         <v>96</v>
@@ -1895,10 +1924,10 @@
         <v>340</v>
       </c>
       <c r="B39" s="2">
-        <v>1494</v>
+        <v>1508</v>
       </c>
       <c r="C39" s="2">
-        <v>11400</v>
+        <v>11498</v>
       </c>
       <c r="D39" t="s">
         <v>96</v>
@@ -1946,10 +1975,10 @@
         <v>8945</v>
       </c>
       <c r="B42" s="2">
-        <v>54569</v>
+        <v>54604</v>
       </c>
       <c r="C42" s="2">
-        <v>371825</v>
+        <v>372070</v>
       </c>
       <c r="D42" t="s">
         <v>96</v>
@@ -1980,10 +2009,10 @@
         <v>143</v>
       </c>
       <c r="B44" s="2">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="C44" s="2">
-        <v>3552</v>
+        <v>3601</v>
       </c>
       <c r="D44" t="s">
         <v>97</v>
@@ -2011,13 +2040,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>35156</v>
+        <v>35253</v>
       </c>
       <c r="B46" s="2">
-        <v>193513</v>
+        <v>194457</v>
       </c>
       <c r="C46" s="2">
-        <v>1343782</v>
+        <v>1350782</v>
       </c>
       <c r="D46" t="s">
         <v>97</v>
@@ -2045,13 +2074,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>2072</v>
+        <v>2080</v>
       </c>
       <c r="B48" s="2">
-        <v>10232</v>
+        <v>10297</v>
       </c>
       <c r="C48" s="2">
-        <v>69783</v>
+        <v>70189</v>
       </c>
       <c r="D48" t="s">
         <v>97</v>
@@ -2065,10 +2094,10 @@
         <v>9918</v>
       </c>
       <c r="B49" s="2">
-        <v>46890</v>
+        <v>46904</v>
       </c>
       <c r="C49" s="2">
-        <v>333555</v>
+        <v>333653</v>
       </c>
       <c r="D49" t="s">
         <v>98</v>
@@ -2130,13 +2159,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>50884</v>
+        <v>50994</v>
       </c>
       <c r="B53" s="2">
-        <v>283916</v>
+        <v>284939</v>
       </c>
       <c r="C53" s="2">
-        <v>1987929</v>
+        <v>1995379</v>
       </c>
       <c r="D53" t="s">
         <v>98</v>
@@ -2167,10 +2196,10 @@
         <v>691</v>
       </c>
       <c r="B55" s="2">
-        <v>3282</v>
+        <v>3303</v>
       </c>
       <c r="C55" s="2">
-        <v>25025</v>
+        <v>25172</v>
       </c>
       <c r="D55" t="s">
         <v>98</v>
@@ -2184,10 +2213,10 @@
         <v>531</v>
       </c>
       <c r="B56" s="2">
-        <v>1938</v>
+        <v>1945</v>
       </c>
       <c r="C56" s="2">
-        <v>17540</v>
+        <v>17589</v>
       </c>
       <c r="D56" t="s">
         <v>98</v>
@@ -2252,10 +2281,10 @@
         <v>1657</v>
       </c>
       <c r="B60" s="2">
-        <v>9520</v>
+        <v>9534</v>
       </c>
       <c r="C60" s="2">
-        <v>66282</v>
+        <v>66380</v>
       </c>
       <c r="D60" t="s">
         <v>98</v>
@@ -2269,10 +2298,10 @@
         <v>9355</v>
       </c>
       <c r="B61" s="2">
-        <v>43919</v>
+        <v>43933</v>
       </c>
       <c r="C61" s="2">
-        <v>313294</v>
+        <v>313392</v>
       </c>
       <c r="D61" t="s">
         <v>103</v>
@@ -2303,10 +2332,10 @@
         <v>244</v>
       </c>
       <c r="B63" s="2">
-        <v>1046</v>
+        <v>1053</v>
       </c>
       <c r="C63" s="2">
-        <v>7330</v>
+        <v>7379</v>
       </c>
       <c r="D63" t="s">
         <v>103</v>
@@ -2334,13 +2363,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>47238</v>
+        <v>47337</v>
       </c>
       <c r="B65" s="2">
-        <v>261452</v>
+        <v>262384</v>
       </c>
       <c r="C65" s="2">
-        <v>1827413</v>
+        <v>1834233</v>
       </c>
       <c r="D65" t="s">
         <v>103</v>
@@ -2371,10 +2400,10 @@
         <v>174</v>
       </c>
       <c r="B67" s="2">
-        <v>793</v>
+        <v>807</v>
       </c>
       <c r="C67" s="2">
-        <v>6027</v>
+        <v>6125</v>
       </c>
       <c r="D67" t="s">
         <v>103</v>
@@ -2388,10 +2417,10 @@
         <v>438</v>
       </c>
       <c r="B68" s="2">
-        <v>2692</v>
+        <v>2706</v>
       </c>
       <c r="C68" s="2">
-        <v>16755</v>
+        <v>16853</v>
       </c>
       <c r="D68" t="s">
         <v>103</v>
@@ -2405,10 +2434,10 @@
         <v>2568</v>
       </c>
       <c r="B69" s="2">
-        <v>13207</v>
+        <v>13235</v>
       </c>
       <c r="C69" s="2">
-        <v>98485</v>
+        <v>98681</v>
       </c>
       <c r="D69" t="s">
         <v>103</v>
@@ -2419,13 +2448,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>9720</v>
+        <v>9724</v>
       </c>
       <c r="B70" s="2">
-        <v>46522</v>
+        <v>46541</v>
       </c>
       <c r="C70" s="2">
-        <v>328895</v>
+        <v>329009</v>
       </c>
       <c r="D70" t="s">
         <v>106</v>
@@ -2470,13 +2499,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>48494</v>
+        <v>48605</v>
       </c>
       <c r="B73" s="2">
-        <v>271336</v>
+        <v>271938</v>
       </c>
       <c r="C73" s="2">
-        <v>1877281</v>
+        <v>1883911</v>
       </c>
       <c r="D73" t="s">
         <v>106</v>
@@ -2507,10 +2536,10 @@
         <v>1297</v>
       </c>
       <c r="B75" s="2">
-        <v>6914</v>
+        <v>6942</v>
       </c>
       <c r="C75" s="2">
-        <v>47155</v>
+        <v>47351</v>
       </c>
       <c r="D75" t="s">
         <v>106</v>
@@ -2524,10 +2553,10 @@
         <v>1616</v>
       </c>
       <c r="B76" s="2">
-        <v>9710</v>
+        <v>9717</v>
       </c>
       <c r="C76" s="2">
-        <v>74626</v>
+        <v>74675</v>
       </c>
       <c r="D76" t="s">
         <v>107</v>
@@ -2541,10 +2570,10 @@
         <v>1556</v>
       </c>
       <c r="B77" s="2">
-        <v>9249</v>
+        <v>9256</v>
       </c>
       <c r="C77" s="2">
-        <v>70677</v>
+        <v>70726</v>
       </c>
       <c r="D77" t="s">
         <v>107</v>
@@ -2558,10 +2587,10 @@
         <v>1550</v>
       </c>
       <c r="B78" s="2">
-        <v>9012</v>
+        <v>9019</v>
       </c>
       <c r="C78" s="2">
-        <v>69391</v>
+        <v>69440</v>
       </c>
       <c r="D78" t="s">
         <v>107</v>
@@ -2575,10 +2604,10 @@
         <v>1434</v>
       </c>
       <c r="B79" s="2">
-        <v>8618</v>
+        <v>8625</v>
       </c>
       <c r="C79" s="2">
-        <v>65641</v>
+        <v>65690</v>
       </c>
       <c r="D79" t="s">
         <v>107</v>
@@ -2592,10 +2621,10 @@
         <v>1663</v>
       </c>
       <c r="B80" s="2">
-        <v>10100</v>
+        <v>10107</v>
       </c>
       <c r="C80" s="2">
-        <v>77469</v>
+        <v>77518</v>
       </c>
       <c r="D80" t="s">
         <v>107</v>
@@ -2623,13 +2652,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>37447</v>
+        <v>37594</v>
       </c>
       <c r="B82" s="2">
-        <v>210618</v>
+        <v>212006</v>
       </c>
       <c r="C82" s="2">
-        <v>1470875</v>
+        <v>1480519</v>
       </c>
       <c r="D82" t="s">
         <v>107</v>
@@ -2643,10 +2672,10 @@
         <v>1405</v>
       </c>
       <c r="B83" s="2">
-        <v>8665</v>
+        <v>8672</v>
       </c>
       <c r="C83" s="2">
-        <v>65597</v>
+        <v>65646</v>
       </c>
       <c r="D83" t="s">
         <v>107</v>
@@ -2660,10 +2689,10 @@
         <v>1795</v>
       </c>
       <c r="B84" s="2">
-        <v>10264</v>
+        <v>10271</v>
       </c>
       <c r="C84" s="2">
-        <v>79349</v>
+        <v>79398</v>
       </c>
       <c r="D84" t="s">
         <v>107</v>
@@ -2677,10 +2706,10 @@
         <v>1594</v>
       </c>
       <c r="B85" s="2">
-        <v>9451</v>
+        <v>9458</v>
       </c>
       <c r="C85" s="2">
-        <v>72590</v>
+        <v>72639</v>
       </c>
       <c r="D85" t="s">
         <v>107</v>
@@ -2694,10 +2723,10 @@
         <v>1599</v>
       </c>
       <c r="B86" s="2">
-        <v>9448</v>
+        <v>9455</v>
       </c>
       <c r="C86" s="2">
-        <v>72692</v>
+        <v>72741</v>
       </c>
       <c r="D86" t="s">
         <v>107</v>
@@ -2728,10 +2757,10 @@
         <v>1482</v>
       </c>
       <c r="B88" s="2">
-        <v>9267</v>
+        <v>9274</v>
       </c>
       <c r="C88" s="2">
-        <v>70191</v>
+        <v>70240</v>
       </c>
       <c r="D88" t="s">
         <v>107</v>
@@ -2745,10 +2774,10 @@
         <v>1647</v>
       </c>
       <c r="B89" s="2">
-        <v>9605</v>
+        <v>9612</v>
       </c>
       <c r="C89" s="2">
-        <v>73766</v>
+        <v>73815</v>
       </c>
       <c r="D89" t="s">
         <v>107</v>
@@ -2762,10 +2791,10 @@
         <v>1698</v>
       </c>
       <c r="B90" s="2">
-        <v>9782</v>
+        <v>9789</v>
       </c>
       <c r="C90" s="2">
-        <v>75473</v>
+        <v>75522</v>
       </c>
       <c r="D90" t="s">
         <v>107</v>
@@ -2779,10 +2808,10 @@
         <v>1692</v>
       </c>
       <c r="B91" s="2">
-        <v>9741</v>
+        <v>9748</v>
       </c>
       <c r="C91" s="2">
-        <v>74952</v>
+        <v>75001</v>
       </c>
       <c r="D91" t="s">
         <v>107</v>
@@ -2796,10 +2825,10 @@
         <v>1551</v>
       </c>
       <c r="B92" s="2">
-        <v>9023</v>
+        <v>9030</v>
       </c>
       <c r="C92" s="2">
-        <v>69487</v>
+        <v>69536</v>
       </c>
       <c r="D92" t="s">
         <v>107</v>
@@ -2813,10 +2842,10 @@
         <v>1641</v>
       </c>
       <c r="B93" s="2">
-        <v>9571</v>
+        <v>9578</v>
       </c>
       <c r="C93" s="2">
-        <v>73718</v>
+        <v>73767</v>
       </c>
       <c r="D93" t="s">
         <v>107</v>
@@ -2830,10 +2859,10 @@
         <v>1707</v>
       </c>
       <c r="B94" s="2">
-        <v>6030</v>
+        <v>6037</v>
       </c>
       <c r="C94" s="2">
-        <v>42096</v>
+        <v>42145</v>
       </c>
       <c r="D94" t="s">
         <v>107</v>
@@ -2844,13 +2873,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>29437</v>
+        <v>29443</v>
       </c>
       <c r="B95" s="2">
-        <v>140908</v>
+        <v>141015</v>
       </c>
       <c r="C95" s="2">
-        <v>1009605</v>
+        <v>1010351</v>
       </c>
       <c r="D95" t="s">
         <v>107</v>
@@ -2861,13 +2890,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>38765</v>
+        <v>38776</v>
       </c>
       <c r="B96" s="2">
-        <v>204807</v>
+        <v>204966</v>
       </c>
       <c r="C96" s="2">
-        <v>1447681</v>
+        <v>1448803</v>
       </c>
       <c r="D96" t="s">
         <v>107</v>
@@ -2881,10 +2910,10 @@
         <v>4901</v>
       </c>
       <c r="B97" s="2">
-        <v>27944</v>
+        <v>27965</v>
       </c>
       <c r="C97" s="2">
-        <v>198955</v>
+        <v>199102</v>
       </c>
       <c r="D97" t="s">
         <v>112</v>
@@ -2898,10 +2927,10 @@
         <v>403</v>
       </c>
       <c r="B98" s="2">
-        <v>1884</v>
+        <v>1891</v>
       </c>
       <c r="C98" s="2">
-        <v>14021</v>
+        <v>14070</v>
       </c>
       <c r="D98" t="s">
         <v>107</v>
@@ -2932,10 +2961,10 @@
         <v>1508</v>
       </c>
       <c r="B100" s="2">
-        <v>9038</v>
+        <v>9045</v>
       </c>
       <c r="C100" s="2">
-        <v>69043</v>
+        <v>69092</v>
       </c>
       <c r="D100" t="s">
         <v>107</v>
@@ -2946,13 +2975,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>60170</v>
+        <v>60268</v>
       </c>
       <c r="B101" s="2">
-        <v>314731</v>
+        <v>315656</v>
       </c>
       <c r="C101" s="2">
-        <v>2216126</v>
+        <v>2222891</v>
       </c>
       <c r="D101" t="s">
         <v>112</v>
@@ -2966,10 +2995,10 @@
         <v>1471</v>
       </c>
       <c r="B102" s="2">
-        <v>8729</v>
+        <v>8736</v>
       </c>
       <c r="C102" s="2">
-        <v>66742</v>
+        <v>66791</v>
       </c>
       <c r="D102" t="s">
         <v>107</v>
@@ -2983,10 +3012,10 @@
         <v>1588</v>
       </c>
       <c r="B103" s="2">
-        <v>9303</v>
+        <v>9310</v>
       </c>
       <c r="C103" s="2">
-        <v>71583</v>
+        <v>71632</v>
       </c>
       <c r="D103" t="s">
         <v>107</v>
@@ -3000,10 +3029,10 @@
         <v>1636</v>
       </c>
       <c r="B104" s="2">
-        <v>9537</v>
+        <v>9544</v>
       </c>
       <c r="C104" s="2">
-        <v>73208</v>
+        <v>73257</v>
       </c>
       <c r="D104" t="s">
         <v>107</v>
@@ -3017,10 +3046,10 @@
         <v>1725</v>
       </c>
       <c r="B105" s="2">
-        <v>9987</v>
+        <v>9994</v>
       </c>
       <c r="C105" s="2">
-        <v>76979</v>
+        <v>77028</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -3031,13 +3060,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>3394</v>
+        <v>3403</v>
       </c>
       <c r="B106" s="2">
-        <v>17589</v>
+        <v>17693</v>
       </c>
       <c r="C106" s="2">
-        <v>125000</v>
+        <v>125692</v>
       </c>
       <c r="D106" t="s">
         <v>107</v>
@@ -3051,10 +3080,10 @@
         <v>1574</v>
       </c>
       <c r="B107" s="2">
-        <v>9367</v>
+        <v>9374</v>
       </c>
       <c r="C107" s="2">
-        <v>71966</v>
+        <v>72015</v>
       </c>
       <c r="D107" t="s">
         <v>107</v>
@@ -3068,10 +3097,10 @@
         <v>1559</v>
       </c>
       <c r="B108" s="2">
-        <v>9434</v>
+        <v>9441</v>
       </c>
       <c r="C108" s="2">
-        <v>71998</v>
+        <v>72047</v>
       </c>
       <c r="D108" t="s">
         <v>107</v>
@@ -3085,10 +3114,10 @@
         <v>1481</v>
       </c>
       <c r="B109" s="2">
-        <v>8920</v>
+        <v>8927</v>
       </c>
       <c r="C109" s="2">
-        <v>68022</v>
+        <v>68071</v>
       </c>
       <c r="D109" t="s">
         <v>107</v>
@@ -3116,13 +3145,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>20102</v>
+        <v>20103</v>
       </c>
       <c r="B111" s="2">
-        <v>113356</v>
+        <v>113384</v>
       </c>
       <c r="C111" s="2">
-        <v>795201</v>
+        <v>795374</v>
       </c>
       <c r="D111" t="s">
         <v>108</v>
@@ -3136,10 +3165,10 @@
         <v>15370</v>
       </c>
       <c r="B112" s="2">
-        <v>85452</v>
+        <v>85459</v>
       </c>
       <c r="C112" s="2">
-        <v>596941</v>
+        <v>596990</v>
       </c>
       <c r="D112" t="s">
         <v>108</v>
@@ -3153,10 +3182,10 @@
         <v>3454</v>
       </c>
       <c r="B113" s="2">
-        <v>23676</v>
+        <v>23683</v>
       </c>
       <c r="C113" s="2">
-        <v>140245</v>
+        <v>140294</v>
       </c>
       <c r="D113" t="s">
         <v>108</v>
@@ -3170,10 +3199,10 @@
         <v>2819</v>
       </c>
       <c r="B114" s="2">
-        <v>21261</v>
+        <v>21268</v>
       </c>
       <c r="C114" s="2">
-        <v>117848</v>
+        <v>117897</v>
       </c>
       <c r="D114" t="s">
         <v>108</v>
@@ -3187,10 +3216,10 @@
         <v>14703</v>
       </c>
       <c r="B115" s="2">
-        <v>90563</v>
+        <v>90581</v>
       </c>
       <c r="C115" s="2">
-        <v>626359</v>
+        <v>626449</v>
       </c>
       <c r="D115" t="s">
         <v>108</v>
@@ -3201,13 +3230,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>24513</v>
+        <v>24613</v>
       </c>
       <c r="B116" s="2">
-        <v>142119</v>
+        <v>143017</v>
       </c>
       <c r="C116" s="2">
-        <v>982790</v>
+        <v>989387</v>
       </c>
       <c r="D116" t="s">
         <v>108</v>
@@ -3221,10 +3250,10 @@
         <v>18766</v>
       </c>
       <c r="B117" s="2">
-        <v>70566</v>
+        <v>70573</v>
       </c>
       <c r="C117" s="2">
-        <v>509682</v>
+        <v>509731</v>
       </c>
       <c r="D117" t="s">
         <v>108</v>
@@ -3238,10 +3267,10 @@
         <v>7799</v>
       </c>
       <c r="B118" s="2">
-        <v>47719</v>
+        <v>47726</v>
       </c>
       <c r="C118" s="2">
-        <v>310412</v>
+        <v>310461</v>
       </c>
       <c r="D118" t="s">
         <v>108</v>
@@ -3252,13 +3281,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>6373</v>
+        <v>6374</v>
       </c>
       <c r="B119" s="2">
-        <v>26970</v>
+        <v>27024</v>
       </c>
       <c r="C119" s="2">
-        <v>210083</v>
+        <v>210449</v>
       </c>
       <c r="D119" t="s">
         <v>108</v>
@@ -3272,10 +3301,10 @@
         <v>87</v>
       </c>
       <c r="B120" s="2">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="C120" s="2">
-        <v>2974</v>
+        <v>3023</v>
       </c>
       <c r="D120" t="s">
         <v>108</v>
@@ -3286,239 +3315,290 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>43729</v>
+        <v>38</v>
       </c>
       <c r="B121" s="2">
-        <v>226939</v>
+        <v>178</v>
       </c>
       <c r="C121" s="2">
-        <v>1676643</v>
+        <v>1593</v>
       </c>
       <c r="D121" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E121" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>4057</v>
+        <v>31407</v>
       </c>
       <c r="B122" s="2">
-        <v>23760</v>
+        <v>178126</v>
       </c>
       <c r="C122" s="2">
-        <v>177234</v>
+        <v>1248656</v>
       </c>
       <c r="D122" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E122" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>4252</v>
+        <v>43728</v>
       </c>
       <c r="B123" s="2">
-        <v>23482</v>
+        <v>227075</v>
       </c>
       <c r="C123" s="2">
-        <v>182662</v>
+        <v>1677469</v>
       </c>
       <c r="D123" t="s">
         <v>109</v>
       </c>
       <c r="E123" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>2839</v>
+        <v>4062</v>
       </c>
       <c r="B124" s="2">
-        <v>21250</v>
+        <v>23798</v>
       </c>
       <c r="C124" s="2">
-        <v>141291</v>
+        <v>177505</v>
       </c>
       <c r="D124" t="s">
         <v>109</v>
       </c>
       <c r="E124" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>4143</v>
+        <v>4257</v>
       </c>
       <c r="B125" s="2">
-        <v>23702</v>
+        <v>23517</v>
       </c>
       <c r="C125" s="2">
-        <v>176613</v>
+        <v>182935</v>
       </c>
       <c r="D125" t="s">
         <v>109</v>
       </c>
       <c r="E125" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>4048</v>
+        <v>2844</v>
       </c>
       <c r="B126" s="2">
-        <v>23552</v>
+        <v>21289</v>
       </c>
       <c r="C126" s="2">
-        <v>175100</v>
+        <v>141571</v>
       </c>
       <c r="D126" t="s">
         <v>109</v>
       </c>
       <c r="E126" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>83</v>
+        <v>4148</v>
       </c>
       <c r="B127" s="2">
-        <v>338</v>
+        <v>23739</v>
       </c>
       <c r="C127" s="2">
-        <v>3765</v>
+        <v>176882</v>
       </c>
       <c r="D127" t="s">
         <v>109</v>
       </c>
       <c r="E127" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>4184</v>
+        <v>4053</v>
       </c>
       <c r="B128" s="2">
-        <v>24090</v>
+        <v>23590</v>
       </c>
       <c r="C128" s="2">
-        <v>179462</v>
+        <v>175370</v>
       </c>
       <c r="D128" t="s">
         <v>109</v>
       </c>
       <c r="E128" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>274</v>
+        <v>87</v>
       </c>
       <c r="B129" s="2">
-        <v>1736</v>
+        <v>357</v>
       </c>
       <c r="C129" s="2">
-        <v>10228</v>
+        <v>3923</v>
       </c>
       <c r="D129" t="s">
         <v>109</v>
       </c>
       <c r="E129" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>1</v>
+        <v>4189</v>
       </c>
       <c r="B130" s="2">
-        <v>1</v>
+        <v>24128</v>
       </c>
       <c r="C130" s="2">
-        <v>11</v>
+        <v>179735</v>
       </c>
       <c r="D130" t="s">
         <v>109</v>
       </c>
       <c r="E130" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>34</v>
+        <v>278</v>
       </c>
       <c r="B131" s="2">
-        <v>159</v>
+        <v>1761</v>
       </c>
       <c r="C131" s="2">
-        <v>1432</v>
+        <v>10433</v>
       </c>
       <c r="D131" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E131" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
-        <v>31403</v>
+        <v>1</v>
       </c>
       <c r="B132" s="2">
-        <v>178050</v>
+        <v>1</v>
       </c>
       <c r="C132" s="2">
-        <v>1248094</v>
+        <v>11</v>
       </c>
       <c r="D132" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E132" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
-        <v>15079</v>
+        <v>1</v>
       </c>
       <c r="B133" s="2">
-        <v>83051</v>
+        <v>1</v>
       </c>
       <c r="C133" s="2">
-        <v>720970</v>
+        <v>11</v>
       </c>
       <c r="D133" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E133" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
-        <v>173</v>
+        <v>40975</v>
       </c>
       <c r="B134" s="2">
-        <v>608</v>
+        <v>239203</v>
       </c>
       <c r="C134" s="2">
-        <v>5900</v>
+        <v>1771063</v>
       </c>
       <c r="D134" t="s">
+        <v>115</v>
+      </c>
+      <c r="E134" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" s="2">
+        <v>44</v>
+      </c>
+      <c r="B135" s="2">
+        <v>176</v>
+      </c>
+      <c r="C135" s="2">
+        <v>1462</v>
+      </c>
+      <c r="D135" t="s">
+        <v>115</v>
+      </c>
+      <c r="E135" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="2">
+        <v>15087</v>
+      </c>
+      <c r="B136" s="2">
+        <v>83112</v>
+      </c>
+      <c r="C136" s="2">
+        <v>721387</v>
+      </c>
+      <c r="D136" t="s">
         <v>111</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E136" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" s="2">
+        <v>183</v>
+      </c>
+      <c r="B137" s="2">
+        <v>658</v>
+      </c>
+      <c r="C137" s="2">
+        <v>6256</v>
+      </c>
+      <c r="D137" t="s">
+        <v>111</v>
+      </c>
+      <c r="E137" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3532,10 +3612,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3810105-F70C-6549-8E2A-9ACB8CFD3E2D}">
-  <dimension ref="A1:C134"/>
+  <dimension ref="A1:C137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C135"/>
+      <selection sqref="A1:C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3558,7 +3638,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="B2" t="s">
         <v>94</v>
@@ -3580,7 +3660,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>156732</v>
+        <v>157612</v>
       </c>
       <c r="B4" t="s">
         <v>94</v>
@@ -3602,7 +3682,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>13499</v>
+        <v>13523</v>
       </c>
       <c r="B6" t="s">
         <v>94</v>
@@ -3613,7 +3693,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>3208</v>
+        <v>3214</v>
       </c>
       <c r="B7" t="s">
         <v>95</v>
@@ -3624,7 +3704,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>3402</v>
+        <v>3408</v>
       </c>
       <c r="B8" t="s">
         <v>95</v>
@@ -3646,7 +3726,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>147087</v>
+        <v>147874</v>
       </c>
       <c r="B10" t="s">
         <v>95</v>
@@ -3657,7 +3737,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>3207</v>
+        <v>3213</v>
       </c>
       <c r="B11" t="s">
         <v>95</v>
@@ -3668,7 +3748,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>3059</v>
+        <v>3065</v>
       </c>
       <c r="B12" t="s">
         <v>95</v>
@@ -3679,7 +3759,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>1655</v>
+        <v>1667</v>
       </c>
       <c r="B13" t="s">
         <v>95</v>
@@ -3701,7 +3781,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>3372</v>
+        <v>3378</v>
       </c>
       <c r="B15" t="s">
         <v>95</v>
@@ -3712,7 +3792,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>3216</v>
+        <v>3222</v>
       </c>
       <c r="B16" t="s">
         <v>95</v>
@@ -3723,7 +3803,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>3368</v>
+        <v>3374</v>
       </c>
       <c r="B17" t="s">
         <v>95</v>
@@ -3734,7 +3814,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>3297</v>
+        <v>3327</v>
       </c>
       <c r="B18" t="s">
         <v>95</v>
@@ -3745,7 +3825,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>9657</v>
+        <v>9711</v>
       </c>
       <c r="B19" t="s">
         <v>95</v>
@@ -3756,7 +3836,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>3400</v>
+        <v>3406</v>
       </c>
       <c r="B20" t="s">
         <v>95</v>
@@ -3767,7 +3847,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>2018</v>
+        <v>2024</v>
       </c>
       <c r="B21" t="s">
         <v>95</v>
@@ -3778,7 +3858,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>125439</v>
+        <v>125550</v>
       </c>
       <c r="B22" t="s">
         <v>95</v>
@@ -3789,7 +3869,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>785</v>
+        <v>791</v>
       </c>
       <c r="B23" t="s">
         <v>95</v>
@@ -3811,7 +3891,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>3226</v>
+        <v>3232</v>
       </c>
       <c r="B25" t="s">
         <v>95</v>
@@ -3822,7 +3902,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>3226</v>
+        <v>3232</v>
       </c>
       <c r="B26" t="s">
         <v>95</v>
@@ -3833,7 +3913,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>6134</v>
+        <v>6146</v>
       </c>
       <c r="B27" t="s">
         <v>95</v>
@@ -3844,7 +3924,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>3184</v>
+        <v>3190</v>
       </c>
       <c r="B28" t="s">
         <v>95</v>
@@ -3855,7 +3935,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>3380</v>
+        <v>3386</v>
       </c>
       <c r="B29" t="s">
         <v>95</v>
@@ -3866,7 +3946,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>3400</v>
+        <v>3406</v>
       </c>
       <c r="B30" t="s">
         <v>95</v>
@@ -3877,7 +3957,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>3203</v>
+        <v>3209</v>
       </c>
       <c r="B31" t="s">
         <v>95</v>
@@ -3888,7 +3968,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>3034</v>
+        <v>3040</v>
       </c>
       <c r="B32" t="s">
         <v>95</v>
@@ -3899,7 +3979,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>3061</v>
+        <v>3067</v>
       </c>
       <c r="B33" t="s">
         <v>95</v>
@@ -3921,7 +4001,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B35" t="s">
         <v>96</v>
@@ -3932,7 +4012,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>5051</v>
+        <v>5063</v>
       </c>
       <c r="B36" t="s">
         <v>96</v>
@@ -3954,7 +4034,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>196078</v>
+        <v>196979</v>
       </c>
       <c r="B38" t="s">
         <v>96</v>
@@ -3965,7 +4045,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>1070</v>
+        <v>1082</v>
       </c>
       <c r="B39" t="s">
         <v>96</v>
@@ -3998,7 +4078,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>42324</v>
+        <v>42354</v>
       </c>
       <c r="B42" t="s">
         <v>96</v>
@@ -4020,7 +4100,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
@@ -4042,7 +4122,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>142257</v>
+        <v>143096</v>
       </c>
       <c r="B46" t="s">
         <v>97</v>
@@ -4064,7 +4144,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>7399</v>
+        <v>7451</v>
       </c>
       <c r="B48" t="s">
         <v>97</v>
@@ -4075,7 +4155,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>16359</v>
+        <v>16371</v>
       </c>
       <c r="B49" t="s">
         <v>98</v>
@@ -4119,7 +4199,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>216004</v>
+        <v>216903</v>
       </c>
       <c r="B53" t="s">
         <v>98</v>
@@ -4141,7 +4221,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>2304</v>
+        <v>2322</v>
       </c>
       <c r="B55" t="s">
         <v>98</v>
@@ -4152,7 +4232,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>935</v>
+        <v>941</v>
       </c>
       <c r="B56" t="s">
         <v>98</v>
@@ -4196,7 +4276,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>6071</v>
+        <v>6083</v>
       </c>
       <c r="B60" t="s">
         <v>98</v>
@@ -4207,7 +4287,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>15454</v>
+        <v>15466</v>
       </c>
       <c r="B61" t="s">
         <v>103</v>
@@ -4229,7 +4309,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="B63" t="s">
         <v>103</v>
@@ -4251,7 +4331,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>199825</v>
+        <v>200650</v>
       </c>
       <c r="B65" t="s">
         <v>103</v>
@@ -4273,7 +4353,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>532</v>
+        <v>544</v>
       </c>
       <c r="B67" t="s">
         <v>103</v>
@@ -4284,7 +4364,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>1276</v>
+        <v>1288</v>
       </c>
       <c r="B68" t="s">
         <v>103</v>
@@ -4295,7 +4375,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>9858</v>
+        <v>9882</v>
       </c>
       <c r="B69" t="s">
         <v>103</v>
@@ -4306,7 +4386,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>16163</v>
+        <v>16177</v>
       </c>
       <c r="B70" t="s">
         <v>106</v>
@@ -4339,7 +4419,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>206118</v>
+        <v>207135</v>
       </c>
       <c r="B73" t="s">
         <v>106</v>
@@ -4361,7 +4441,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>5150</v>
+        <v>5174</v>
       </c>
       <c r="B75" t="s">
         <v>106</v>
@@ -4372,7 +4452,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>4439</v>
+        <v>4445</v>
       </c>
       <c r="B76" t="s">
         <v>107</v>
@@ -4383,7 +4463,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>3873</v>
+        <v>3879</v>
       </c>
       <c r="B77" t="s">
         <v>107</v>
@@ -4394,7 +4474,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>3840</v>
+        <v>3846</v>
       </c>
       <c r="B78" t="s">
         <v>107</v>
@@ -4405,7 +4485,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>3551</v>
+        <v>3557</v>
       </c>
       <c r="B79" t="s">
         <v>107</v>
@@ -4416,7 +4496,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>4827</v>
+        <v>4833</v>
       </c>
       <c r="B80" t="s">
         <v>107</v>
@@ -4438,7 +4518,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>163455</v>
+        <v>164693</v>
       </c>
       <c r="B82" t="s">
         <v>107</v>
@@ -4449,7 +4529,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>3468</v>
+        <v>3474</v>
       </c>
       <c r="B83" t="s">
         <v>107</v>
@@ -4460,7 +4540,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>4779</v>
+        <v>4785</v>
       </c>
       <c r="B84" t="s">
         <v>107</v>
@@ -4471,7 +4551,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>4152</v>
+        <v>4158</v>
       </c>
       <c r="B85" t="s">
         <v>107</v>
@@ -4482,7 +4562,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>4187</v>
+        <v>4193</v>
       </c>
       <c r="B86" t="s">
         <v>107</v>
@@ -4504,7 +4584,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>4089</v>
+        <v>4095</v>
       </c>
       <c r="B88" t="s">
         <v>107</v>
@@ -4515,7 +4595,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>4187</v>
+        <v>4193</v>
       </c>
       <c r="B89" t="s">
         <v>107</v>
@@ -4526,7 +4606,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>4532</v>
+        <v>4538</v>
       </c>
       <c r="B90" t="s">
         <v>107</v>
@@ -4537,7 +4617,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>4289</v>
+        <v>4295</v>
       </c>
       <c r="B91" t="s">
         <v>107</v>
@@ -4548,7 +4628,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>3845</v>
+        <v>3851</v>
       </c>
       <c r="B92" t="s">
         <v>107</v>
@@ -4559,7 +4639,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>4119</v>
+        <v>4125</v>
       </c>
       <c r="B93" t="s">
         <v>107</v>
@@ -4570,7 +4650,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>2369</v>
+        <v>2375</v>
       </c>
       <c r="B94" t="s">
         <v>107</v>
@@ -4581,7 +4661,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>95056</v>
+        <v>95150</v>
       </c>
       <c r="B95" t="s">
         <v>107</v>
@@ -4592,7 +4672,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>148713</v>
+        <v>148853</v>
       </c>
       <c r="B96" t="s">
         <v>107</v>
@@ -4603,7 +4683,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>21749</v>
+        <v>21767</v>
       </c>
       <c r="B97" t="s">
         <v>112</v>
@@ -4614,7 +4694,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>912</v>
+        <v>918</v>
       </c>
       <c r="B98" t="s">
         <v>107</v>
@@ -4636,7 +4716,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>3735</v>
+        <v>3741</v>
       </c>
       <c r="B100" t="s">
         <v>107</v>
@@ -4647,7 +4727,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>210127</v>
+        <v>210945</v>
       </c>
       <c r="B101" t="s">
         <v>112</v>
@@ -4658,7 +4738,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>3651</v>
+        <v>3657</v>
       </c>
       <c r="B102" t="s">
         <v>107</v>
@@ -4669,7 +4749,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>3953</v>
+        <v>3959</v>
       </c>
       <c r="B103" t="s">
         <v>107</v>
@@ -4680,7 +4760,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>4121</v>
+        <v>4127</v>
       </c>
       <c r="B104" t="s">
         <v>107</v>
@@ -4691,7 +4771,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>4583</v>
+        <v>4589</v>
       </c>
       <c r="B105" t="s">
         <v>107</v>
@@ -4702,7 +4782,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>13237</v>
+        <v>13321</v>
       </c>
       <c r="B106" t="s">
         <v>107</v>
@@ -4713,7 +4793,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>4093</v>
+        <v>4099</v>
       </c>
       <c r="B107" t="s">
         <v>107</v>
@@ -4724,7 +4804,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>4133</v>
+        <v>4139</v>
       </c>
       <c r="B108" t="s">
         <v>107</v>
@@ -4735,7 +4815,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>3676</v>
+        <v>3682</v>
       </c>
       <c r="B109" t="s">
         <v>107</v>
@@ -4757,7 +4837,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>84949</v>
+        <v>84975</v>
       </c>
       <c r="B111" t="s">
         <v>108</v>
@@ -4768,7 +4848,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>60277</v>
+        <v>60283</v>
       </c>
       <c r="B112" t="s">
         <v>108</v>
@@ -4779,7 +4859,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>5367</v>
+        <v>5373</v>
       </c>
       <c r="B113" t="s">
         <v>108</v>
@@ -4790,7 +4870,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>2228</v>
+        <v>2234</v>
       </c>
       <c r="B114" t="s">
         <v>108</v>
@@ -4801,7 +4881,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>60255</v>
+        <v>60272</v>
       </c>
       <c r="B115" t="s">
         <v>108</v>
@@ -4812,7 +4892,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>109533</v>
+        <v>110329</v>
       </c>
       <c r="B116" t="s">
         <v>108</v>
@@ -4823,7 +4903,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>31560</v>
+        <v>31566</v>
       </c>
       <c r="B117" t="s">
         <v>108</v>
@@ -4834,7 +4914,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>26119</v>
+        <v>26125</v>
       </c>
       <c r="B118" t="s">
         <v>108</v>
@@ -4845,7 +4925,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>19318</v>
+        <v>19365</v>
       </c>
       <c r="B119" t="s">
         <v>108</v>
@@ -4856,7 +4936,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B120" t="s">
         <v>108</v>
@@ -4867,155 +4947,188 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>170098</v>
+        <v>109</v>
       </c>
       <c r="B121" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C121" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>16949</v>
+        <v>133425</v>
       </c>
       <c r="B122" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C122" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>16602</v>
+        <v>170214</v>
       </c>
       <c r="B123" t="s">
         <v>109</v>
       </c>
       <c r="C123" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>14995</v>
+        <v>16980</v>
       </c>
       <c r="B124" t="s">
         <v>109</v>
       </c>
       <c r="C124" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>16974</v>
+        <v>16630</v>
       </c>
       <c r="B125" t="s">
         <v>109</v>
       </c>
       <c r="C125" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>16789</v>
+        <v>15027</v>
       </c>
       <c r="B126" t="s">
         <v>109</v>
       </c>
       <c r="C126" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>106</v>
+        <v>17004</v>
       </c>
       <c r="B127" t="s">
         <v>109</v>
       </c>
       <c r="C127" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>17257</v>
+        <v>16820</v>
       </c>
       <c r="B128" t="s">
         <v>109</v>
       </c>
       <c r="C128" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B129" t="s">
         <v>109</v>
       </c>
       <c r="C129" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>0</v>
+        <v>17288</v>
       </c>
       <c r="B130" t="s">
         <v>109</v>
       </c>
       <c r="C130" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="B131" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C131" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
-        <v>133362</v>
+        <v>0</v>
       </c>
       <c r="B132" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C132" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
-        <v>52571</v>
+        <v>0</v>
       </c>
       <c r="B133" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C133" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
-        <v>390</v>
+        <v>177994</v>
       </c>
       <c r="B134" t="s">
+        <v>115</v>
+      </c>
+      <c r="C134" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="2">
+        <v>115</v>
+      </c>
+      <c r="B135" t="s">
+        <v>115</v>
+      </c>
+      <c r="C135" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="2">
+        <v>52623</v>
+      </c>
+      <c r="B136" t="s">
         <v>111</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C136" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="2">
+        <v>429</v>
+      </c>
+      <c r="B137" t="s">
+        <v>111</v>
+      </c>
+      <c r="C137" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update word count spreadsheet
</commit_message>
<xml_diff>
--- a/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
+++ b/code-analysis/word-count-code-comments/Code-comments-word-counts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mark/Documents/Files/Websites/Repositories/bbcelite-scripts/code-analysis/word-count-code-comments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6755AB8-43A0-C447-B0F7-0647BFADA7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FC01FE-4D66-2045-991A-B77BE1DCB18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="2800" windowWidth="21580" windowHeight="17800" xr2:uid="{F0A95109-ED5E-2247-9F97-3254041D3CDA}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="linecount.txt" sheetId="1" r:id="rId2"/>
     <sheet name="wordcount.txt" sheetId="4" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="121">
   <si>
     <t>Lines</t>
   </si>
@@ -393,6 +396,12 @@
   </si>
   <si>
     <t>the-sentinel-disc.asm</t>
+  </si>
+  <si>
+    <t>Unique commentary word count:</t>
+  </si>
+  <si>
+    <t>Commentary plus deep dives:</t>
   </si>
 </sst>
 </file>
@@ -484,6 +493,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Results"/>
+      <sheetName val="wordcount.txt"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="7">
+          <cell r="B7">
+            <v>428676</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -783,7 +816,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4742C6F-ED5A-B74D-BFAE-09A904247301}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -793,11 +826,12 @@
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -811,12 +845,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="4">
-        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A2,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$I$4</f>
+        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A2,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$G$4</f>
         <v>151589</v>
       </c>
       <c r="C2" s="4">
@@ -827,15 +861,15 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A2)</f>
         <v>800265</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F2" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="4">
+      <c r="G2" s="4">
         <f>58674-54876</f>
         <v>3798</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -851,20 +885,20 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A3)</f>
         <v>623092</v>
       </c>
-      <c r="H3" t="s">
+      <c r="F3" t="s">
         <v>83</v>
       </c>
-      <c r="I3" s="4">
+      <c r="G3" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,"elite-a-beebasm",linecount.txt!E:E,"=elite-ships*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>95</v>
       </c>
       <c r="B4" s="4">
-        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A4,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$I$8</f>
+        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$A4,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")+$G$8</f>
         <v>100991</v>
       </c>
       <c r="C4" s="4">
@@ -875,15 +909,15 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A4)</f>
         <v>544543</v>
       </c>
-      <c r="H4" t="s">
+      <c r="F4" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="4">
-        <f>I2-I3</f>
+      <c r="G4" s="4">
+        <f>G2-G3</f>
         <v>3798</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -899,9 +933,9 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A5)</f>
         <v>369255</v>
       </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -917,15 +951,15 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A6)</f>
         <v>355882</v>
       </c>
-      <c r="H6" t="s">
+      <c r="F6" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="4">
+      <c r="G6" s="4">
         <f>3318- 86-(325 - 213)-(3206 - 3113)</f>
         <v>3027</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -941,15 +975,15 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A7)</f>
         <v>343621</v>
       </c>
-      <c r="H7" t="s">
+      <c r="F7" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="4">
+      <c r="G7" s="4">
         <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,"disc-elite-beebasm",linecount.txt!E:E,"=elite-ships*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -965,15 +999,15 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A8)</f>
         <v>355943</v>
       </c>
-      <c r="H8" t="s">
+      <c r="F8" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="4">
-        <f>I6-I7</f>
+      <c r="G8" s="4">
+        <f>G6-G7</f>
         <v>3027</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -989,9 +1023,9 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A9)</f>
         <v>325822</v>
       </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -1007,12 +1041,12 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A10)</f>
         <v>325884</v>
       </c>
-      <c r="H10" t="s">
+      <c r="F10" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -1028,15 +1062,15 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A11)</f>
         <v>232952</v>
       </c>
-      <c r="H11" t="s">
+      <c r="F11" t="s">
         <v>2</v>
       </c>
-      <c r="I11" s="4">
-        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$H11,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
+      <c r="G11" s="4">
+        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$F11,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -1052,15 +1086,15 @@
         <f>SUMIFS(linecount.txt!B:B,linecount.txt!D:D,Totals!$A12)</f>
         <v>239380</v>
       </c>
-      <c r="H12" t="s">
+      <c r="F12" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="4">
-        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$H12,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
+      <c r="G12" s="4">
+        <f>SUMIFS(linecount.txt!A:A,linecount.txt!D:D,Totals!$F12,linecount.txt!E:E,"&lt;&gt;elite-build-options.asm",linecount.txt!E:E,"&lt;&gt;elite-bank-options.asm",linecount.txt!E:E,"&lt;&gt;elite-disc.asm",linecount.txt!E:E,"&lt;&gt;elite-readme.asm")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -1077,7 +1111,7 @@
         <v>205681</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -1094,7 +1128,7 @@
         <v>178304</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -1111,7 +1145,7 @@
         <v>83770</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="5">
         <f>SUM(B2:B15)</f>
         <v>917273</v>
@@ -1222,7 +1256,7 @@
         <v>169441</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -1230,21 +1264,37 @@
         <v>198227</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C34" s="5">
         <f>SUM(C27:C33)</f>
         <v>1084625</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" s="6">
+        <f>C3+C14+C5+C15+C12</f>
+        <v>1035680</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>93</v>
       </c>
       <c r="C36" s="6">
         <v>835997</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>120</v>
+      </c>
+      <c r="G36" s="6">
+        <f>C16+[1]Results!$B$7</f>
+        <v>3842050</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>92</v>
       </c>

</xml_diff>